<commit_message>
fixed small calc error on backprop spreadsheet
</commit_message>
<xml_diff>
--- a/docs/neural-networks-on-a-spreadsheet.xlsx
+++ b/docs/neural-networks-on-a-spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iandurbach/Dropbox/teaching/STA_dscifi/datasci-fi-pub/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8740C9D7-B1C7-1A4D-8648-8E91C463DB34}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14F559C-1C4E-C645-AAE8-E2B060B25BD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="560" windowWidth="27720" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="560" windowWidth="27720" windowHeight="14940" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="7" r:id="rId1"/>
@@ -26,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ian Durbach</author>
   </authors>
   <commentList>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0">
+    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -88,12 +88,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ian Durbach</author>
   </authors>
   <commentList>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -204,12 +204,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ian Durbach</author>
   </authors>
   <commentList>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -235,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -266,12 +266,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ian Durbach</author>
   </authors>
   <commentList>
-    <comment ref="AO22" authorId="0" shapeId="0">
+    <comment ref="AO22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV22" authorId="0" shapeId="0">
+    <comment ref="AV22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T23" authorId="0" shapeId="0">
+    <comment ref="T23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -367,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U23" authorId="0" shapeId="0">
+    <comment ref="U23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -392,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y23" authorId="0" shapeId="0">
+    <comment ref="Y23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -416,7 +416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO23" authorId="0" shapeId="0">
+    <comment ref="AO23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -440,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA23" authorId="0" shapeId="0">
+    <comment ref="BA23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
       <text>
         <r>
           <rPr>
@@ -926,10 +926,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -1176,13 +1176,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1238,10 +1238,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1881,10 +1881,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1901,7 +1901,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" thickBot="1"/>
-    <row r="3" spans="1:2" ht="65" thickBot="1">
+    <row r="3" spans="1:2" ht="69" thickBot="1">
       <c r="A3" s="36" t="s">
         <v>134</v>
       </c>
@@ -1910,7 +1910,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" thickBot="1"/>
-    <row r="5" spans="1:2" ht="32">
+    <row r="5" spans="1:2" ht="34">
       <c r="A5" s="29" t="s">
         <v>136</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="17">
       <c r="A6" s="38" t="s">
         <v>138</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" thickBot="1">
+    <row r="7" spans="1:2" ht="18" thickBot="1">
       <c r="A7" s="39" t="s">
         <v>140</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="B9" s="28"/>
     </row>
-    <row r="10" spans="1:2" ht="32">
+    <row r="10" spans="1:2" ht="34">
       <c r="A10" s="29" t="s">
         <v>121</v>
       </c>
@@ -1948,13 +1948,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="33" thickBot="1">
+    <row r="11" spans="1:2" ht="35" thickBot="1">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="65" thickBot="1">
+    <row r="12" spans="1:2" ht="69" thickBot="1">
       <c r="A12" s="33" t="s">
         <v>122</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="48">
+    <row r="13" spans="1:2" ht="51">
       <c r="A13" s="29" t="s">
         <v>123</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="49" thickBot="1">
+    <row r="14" spans="1:2" ht="52" thickBot="1">
       <c r="A14" s="35"/>
       <c r="B14" s="32" t="s">
         <v>133</v>
@@ -1984,7 +1984,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="49" thickBot="1">
+    <row r="16" spans="1:2" ht="52" thickBot="1">
       <c r="A16" s="36" t="s">
         <v>124</v>
       </c>
@@ -2000,7 +2000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2795,7 +2795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3648,7 +3648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5276,7 +5276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6636,7 +6636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7999,11 +7999,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BI36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BA23" sqref="BA23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL24" sqref="AL24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8304,86 +8304,86 @@
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="2:61" ht="48" customHeight="1">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="41" t="s">
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42" t="s">
+      <c r="H22" s="42"/>
+      <c r="I22" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="41" t="s">
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="O22" s="41"/>
-      <c r="P22" s="42" t="s">
+      <c r="O22" s="42"/>
+      <c r="P22" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="T22" s="41" t="s">
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="T22" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="U22" s="41"/>
-      <c r="V22" s="41"/>
-      <c r="W22" s="41"/>
-      <c r="Y22" s="41" t="s">
+      <c r="U22" s="42"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="Y22" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="Z22" s="41"/>
-      <c r="AA22" s="41"/>
-      <c r="AB22" s="41"/>
-      <c r="AC22" s="41"/>
-      <c r="AE22" s="41" t="s">
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="42"/>
+      <c r="AB22" s="42"/>
+      <c r="AC22" s="42"/>
+      <c r="AE22" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="AF22" s="41"/>
-      <c r="AG22" s="41"/>
-      <c r="AH22" s="41"/>
-      <c r="AJ22" s="41" t="s">
+      <c r="AF22" s="42"/>
+      <c r="AG22" s="42"/>
+      <c r="AH22" s="42"/>
+      <c r="AJ22" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="AK22" s="41"/>
-      <c r="AL22" s="41"/>
-      <c r="AM22" s="41"/>
-      <c r="AO22" s="41" t="s">
+      <c r="AK22" s="42"/>
+      <c r="AL22" s="42"/>
+      <c r="AM22" s="42"/>
+      <c r="AO22" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="AP22" s="41"/>
-      <c r="AQ22" s="41"/>
-      <c r="AR22" s="41"/>
-      <c r="AS22" s="41"/>
-      <c r="AT22" s="41"/>
-      <c r="AV22" s="41" t="s">
+      <c r="AP22" s="42"/>
+      <c r="AQ22" s="42"/>
+      <c r="AR22" s="42"/>
+      <c r="AS22" s="42"/>
+      <c r="AT22" s="42"/>
+      <c r="AV22" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="AW22" s="41"/>
-      <c r="AX22" s="41"/>
-      <c r="AY22" s="41"/>
-      <c r="BA22" s="41" t="s">
+      <c r="AW22" s="42"/>
+      <c r="AX22" s="42"/>
+      <c r="AY22" s="42"/>
+      <c r="BA22" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="BB22" s="41"/>
-      <c r="BC22" s="41"/>
-      <c r="BD22" s="41"/>
-      <c r="BF22" s="41" t="s">
+      <c r="BB22" s="42"/>
+      <c r="BC22" s="42"/>
+      <c r="BD22" s="42"/>
+      <c r="BF22" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="BG22" s="41"/>
-      <c r="BH22" s="41"/>
-      <c r="BI22" s="41"/>
-    </row>
-    <row r="23" spans="2:61" ht="32">
+      <c r="BG22" s="42"/>
+      <c r="BH22" s="42"/>
+      <c r="BI22" s="42"/>
+    </row>
+    <row r="23" spans="2:61" ht="34">
       <c r="B23" s="13" t="s">
         <v>66</v>
       </c>
@@ -8649,15 +8649,15 @@
         <v>0.39767000000000169</v>
       </c>
       <c r="AF24">
-        <f t="shared" ref="AF24:AF36" si="12">W24*AA24</f>
-        <v>-0.22995900000000585</v>
+        <f>W24*AB24</f>
+        <v>-0.22488637500000264</v>
       </c>
       <c r="AG24">
-        <f t="shared" ref="AG24:AG36" si="13">U24*AB24</f>
-        <v>0.39767000000000169</v>
+        <f>U24*AA24</f>
+        <v>0.40664000000000733</v>
       </c>
       <c r="AH24">
-        <f t="shared" ref="AH24:AH36" si="14">W24*AC24</f>
+        <f t="shared" ref="AH24:AH36" si="12">W24*AC24</f>
         <v>-0.22995900000000585</v>
       </c>
       <c r="AJ24">
@@ -8666,70 +8666,70 @@
       </c>
       <c r="AK24">
         <f>J24-$I$19*AF24</f>
-        <v>0.56497950000000297</v>
+        <v>0.56244318750000133</v>
       </c>
       <c r="AL24">
         <f>K24-$I$19*AG24</f>
-        <v>0.30116499999999913</v>
+        <v>0.29667999999999634</v>
       </c>
       <c r="AM24">
         <f>L24-$I$19*AH24</f>
         <v>0.69497950000000286</v>
       </c>
       <c r="AO24">
-        <f t="shared" ref="AO24:AO36" si="15">U24*I24</f>
+        <f t="shared" ref="AO24:AO36" si="13">U24*I24</f>
         <v>0.47839999999999883</v>
       </c>
       <c r="AP24">
-        <f t="shared" ref="AP24:AP36" si="16">W24*J24</f>
+        <f t="shared" ref="AP24:AP36" si="14">W24*J24</f>
         <v>-0.3043575000000015</v>
       </c>
       <c r="AQ24">
-        <f t="shared" ref="AQ24:AQ36" si="17">AO24+AP24</f>
+        <f t="shared" ref="AQ24:AQ36" si="15">AO24+AP24</f>
         <v>0.17404249999999732</v>
       </c>
       <c r="AR24">
-        <f t="shared" ref="AR24:AR36" si="18">U24*K24</f>
+        <f t="shared" ref="AR24:AR36" si="16">U24*K24</f>
         <v>0.59799999999999853</v>
       </c>
       <c r="AS24">
-        <f t="shared" ref="AS24:AS36" si="19">W24*L24</f>
+        <f t="shared" ref="AS24:AS36" si="17">W24*L24</f>
         <v>-0.39228300000000194</v>
       </c>
       <c r="AT24">
-        <f t="shared" ref="AT24:AT36" si="20">AR24+AS24</f>
+        <f t="shared" ref="AT24:AT36" si="18">AR24+AS24</f>
         <v>0.2057169999999966</v>
       </c>
       <c r="AV24">
-        <f t="shared" ref="AV24:AV36" si="21">$C$19</f>
+        <f t="shared" ref="AV24:AV36" si="19">$C$19</f>
         <v>0.05</v>
       </c>
       <c r="AW24">
-        <f t="shared" ref="AW24:AW36" si="22">$C$20</f>
+        <f t="shared" ref="AW24:AW36" si="20">$C$20</f>
         <v>0.1</v>
       </c>
       <c r="AX24">
-        <f t="shared" ref="AX24:AX36" si="23">$C$19</f>
+        <f t="shared" ref="AX24:AX36" si="21">$C$19</f>
         <v>0.05</v>
       </c>
       <c r="AY24">
-        <f t="shared" ref="AY24:AY36" si="24">$C$20</f>
+        <f t="shared" ref="AY24:AY36" si="22">$C$20</f>
         <v>0.1</v>
       </c>
       <c r="BA24" s="4">
-        <f t="shared" ref="BA24:BA36" si="25">AQ24*AV24</f>
+        <f t="shared" ref="BA24:BA36" si="23">AQ24*AV24</f>
         <v>8.7021249999998662E-3</v>
       </c>
       <c r="BB24" s="4">
-        <f t="shared" ref="BB24:BB36" si="26">AT24*AX24</f>
+        <f t="shared" ref="BB24:BB36" si="24">AT24*AX24</f>
         <v>1.0285849999999831E-2</v>
       </c>
       <c r="BC24" s="4">
-        <f t="shared" ref="BC24:BC36" si="27">AQ24*AW24</f>
+        <f t="shared" ref="BC24:BC36" si="25">AQ24*AW24</f>
         <v>1.7404249999999732E-2</v>
       </c>
       <c r="BD24" s="4">
-        <f t="shared" ref="BD24:BD36" si="28">AT24*AY24</f>
+        <f t="shared" ref="BD24:BD36" si="26">AT24*AY24</f>
         <v>2.0571699999999662E-2</v>
       </c>
       <c r="BE24" s="4"/>
@@ -8752,19 +8752,19 @@
     </row>
     <row r="25" spans="2:61">
       <c r="B25" s="19">
-        <f t="shared" ref="B25:E36" si="29">BF24</f>
+        <f t="shared" ref="B25:E36" si="27">BF24</f>
         <v>0.14564893750000008</v>
       </c>
       <c r="C25" s="19">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>0.1948570750000001</v>
       </c>
       <c r="D25" s="19">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>0.24129787500000013</v>
       </c>
       <c r="E25" s="19">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>0.28971415000000017</v>
       </c>
       <c r="F25" s="20">
@@ -8772,7 +8772,7 @@
         <v>0.3</v>
       </c>
       <c r="G25" s="21">
-        <f t="shared" ref="G25:G36" si="30">B25*$C$19+D25*$C$20+F25</f>
+        <f t="shared" ref="G25:G36" si="28">B25*$C$19+D25*$C$20+F25</f>
         <v>0.331412234375</v>
       </c>
       <c r="H25" s="21">
@@ -8780,2515 +8780,2510 @@
         <v>0.33871426874999999</v>
       </c>
       <c r="I25" s="19">
-        <f t="shared" ref="I25:L36" si="31">AJ24</f>
+        <f t="shared" ref="I25:L36" si="29">AJ24</f>
         <v>0.20116499999999918</v>
       </c>
       <c r="J25" s="19">
-        <f t="shared" si="31"/>
-        <v>0.56497950000000297</v>
+        <f t="shared" si="29"/>
+        <v>0.56244318750000133</v>
       </c>
       <c r="K25" s="19">
-        <f t="shared" si="31"/>
-        <v>0.30116499999999913</v>
+        <f t="shared" si="29"/>
+        <v>0.29667999999999634</v>
       </c>
       <c r="L25" s="19">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>0.69497950000000286</v>
       </c>
       <c r="M25" s="20">
-        <f t="shared" ref="M25:M36" si="32">M24</f>
+        <f t="shared" ref="M25:M36" si="30">M24</f>
         <v>0.3</v>
       </c>
       <c r="N25" s="21">
         <f t="shared" si="1"/>
-        <v>0.46867742487614006</v>
+        <v>0.46715829138079534</v>
       </c>
       <c r="O25" s="21">
         <f t="shared" si="2"/>
-        <v>0.72264059160981287</v>
+        <v>0.72180002661711407</v>
       </c>
       <c r="P25" s="22">
         <f t="shared" si="3"/>
-        <v>0.21038498009100709</v>
+        <v>0.20899370337820816</v>
       </c>
       <c r="Q25" s="22">
         <f t="shared" si="4"/>
-        <v>7.1481053254750862E-2</v>
+        <v>7.1931225722580719E-2</v>
       </c>
       <c r="R25" s="22">
         <f t="shared" si="5"/>
-        <v>0.28186603334575794</v>
+        <v>0.28092492910078887</v>
       </c>
       <c r="T25">
         <f t="shared" si="6"/>
-        <v>0.29113958184328076</v>
+        <v>0.29016809492840479</v>
       </c>
       <c r="U25">
         <f t="shared" si="7"/>
-        <v>0.92735484975228211</v>
+        <v>0.92431658276159179</v>
       </c>
       <c r="V25">
         <f t="shared" si="8"/>
-        <v>0.27661884517795421</v>
+        <v>0.27566092963313116</v>
       </c>
       <c r="W25">
         <f t="shared" si="9"/>
-        <v>-0.52471881678037291</v>
+        <v>-0.52639994676577095</v>
       </c>
       <c r="Y25">
         <f t="shared" si="10"/>
-        <v>0.47199154721989006</v>
+        <v>0.47047241372454535</v>
       </c>
       <c r="Z25">
-        <f t="shared" ref="Z25:Z36" si="33">(Y25-N25)/0.01</f>
+        <f t="shared" ref="Z25:Z36" si="31">(Y25-N25)/0.01</f>
         <v>0.33141223437500034</v>
       </c>
       <c r="AA25">
-        <f t="shared" ref="AA25:AA36" si="34">((I25*G25+(K25+0.01)*H25+M25)-N25)/0.01</f>
-        <v>0.33871426874999555</v>
+        <f t="shared" ref="AA25:AA36" si="32">((I25*G25+(K25+0.01)*H25+M25)-N25)/0.01</f>
+        <v>0.3387142687500011</v>
       </c>
       <c r="AB25">
-        <f t="shared" ref="AB25:AB36" si="35">(((J25+0.01)*G25+L25*H25+M25)-O25)/0.01</f>
+        <f t="shared" ref="AB25:AB36" si="33">(((J25+0.01)*G25+L25*H25+M25)-O25)/0.01</f>
         <v>0.33141223437500589</v>
       </c>
       <c r="AC25">
-        <f t="shared" ref="AC25:AC36" si="36">((J25*G25+(L25+0.01)*H25+M25)-O25)/0.01</f>
+        <f t="shared" ref="AC25:AC36" si="34">((J25*G25+(L25+0.01)*H25+M25)-O25)/0.01</f>
         <v>0.33871426875000665</v>
       </c>
       <c r="AE25">
         <f t="shared" si="11"/>
-        <v>0.30733674281489654</v>
+        <v>0.30632982396288405</v>
       </c>
       <c r="AF25">
+        <f t="shared" ref="AF25:AF36" si="35">W25*AB25</f>
+        <v>-0.17445538253252832</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" ref="AG25:AG36" si="36">U25*AA25</f>
+        <v>0.31307921542359246</v>
+      </c>
+      <c r="AH25">
         <f t="shared" si="12"/>
-        <v>-0.17772975032512692</v>
-      </c>
-      <c r="AG25">
-        <f t="shared" si="13"/>
-        <v>0.3073367428149017</v>
-      </c>
-      <c r="AH25">
-        <f t="shared" si="14"/>
-        <v>-0.17772975032513272</v>
+        <v>-0.17829917303881054</v>
       </c>
       <c r="AJ25">
         <f t="shared" ref="AJ25:AJ36" si="37">I25-$I$19*AE25</f>
-        <v>4.749662859255091E-2</v>
+        <v>4.8000088018557152E-2</v>
       </c>
       <c r="AK25">
         <f t="shared" ref="AK25:AK36" si="38">J25-$I$19*AF25</f>
-        <v>0.65384437516256644</v>
+        <v>0.6496708787662655</v>
       </c>
       <c r="AL25">
         <f t="shared" ref="AL25:AL36" si="39">K25-$I$19*AG25</f>
-        <v>0.14749662859254828</v>
+        <v>0.14014039228820011</v>
       </c>
       <c r="AM25">
         <f t="shared" ref="AM25:AM36" si="40">L25-$I$19*AH25</f>
-        <v>0.78384437516256922</v>
+        <v>0.78412908651940816</v>
       </c>
       <c r="AO25">
+        <f t="shared" si="13"/>
+        <v>0.18594014537123485</v>
+      </c>
+      <c r="AP25">
+        <f t="shared" si="14"/>
+        <v>-0.29607006395877122</v>
+      </c>
+      <c r="AQ25">
         <f t="shared" si="15"/>
-        <v>0.18655133835041707</v>
-      </c>
-      <c r="AP25">
+        <v>-0.11012991858753637</v>
+      </c>
+      <c r="AR25">
         <f t="shared" si="16"/>
-        <v>-0.29645537474516825</v>
-      </c>
-      <c r="AQ25">
+        <v>0.27422624377370569</v>
+      </c>
+      <c r="AS25">
         <f t="shared" si="17"/>
-        <v>-0.10990403639475119</v>
-      </c>
-      <c r="AR25">
+        <v>-0.36583717180330361</v>
+      </c>
+      <c r="AT25">
         <f t="shared" si="18"/>
-        <v>0.27928682332564525</v>
-      </c>
-      <c r="AS25">
+        <v>-9.1610928029597916E-2</v>
+      </c>
+      <c r="AV25">
         <f t="shared" si="19"/>
-        <v>-0.36466882092661668</v>
-      </c>
-      <c r="AT25">
+        <v>0.05</v>
+      </c>
+      <c r="AW25">
         <f t="shared" si="20"/>
-        <v>-8.5381997600971427E-2</v>
-      </c>
-      <c r="AV25">
+        <v>0.1</v>
+      </c>
+      <c r="AX25">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW25">
+      <c r="AY25">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX25">
+      <c r="BA25" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY25">
+        <v>-5.5064959293768187E-3</v>
+      </c>
+      <c r="BB25" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA25" s="4">
+        <v>-4.5805464014798958E-3</v>
+      </c>
+      <c r="BC25" s="4">
         <f t="shared" si="25"/>
-        <v>-5.4952018197375599E-3</v>
-      </c>
-      <c r="BB25" s="4">
+        <v>-1.1012991858753637E-2</v>
+      </c>
+      <c r="BD25" s="4">
         <f t="shared" si="26"/>
-        <v>-4.2690998800485715E-3</v>
-      </c>
-      <c r="BC25" s="4">
-        <f t="shared" si="27"/>
-        <v>-1.099040363947512E-2</v>
-      </c>
-      <c r="BD25" s="4">
-        <f t="shared" si="28"/>
-        <v>-8.538199760097143E-3</v>
+        <v>-9.1610928029597916E-3</v>
       </c>
       <c r="BE25" s="4"/>
       <c r="BF25" s="4">
         <f t="shared" ref="BF25:BF36" si="41">B25-$I$19*BA25</f>
-        <v>0.14839653840986886</v>
+        <v>0.14840218546468847</v>
       </c>
       <c r="BG25" s="4">
         <f t="shared" ref="BG25:BG36" si="42">C25-$I$19*BB25</f>
-        <v>0.1969916249400244</v>
+        <v>0.19714734820074004</v>
       </c>
       <c r="BH25" s="4">
         <f t="shared" ref="BH25:BH36" si="43">D25-$I$19*BC25</f>
-        <v>0.24679307681973769</v>
+        <v>0.24680437092937696</v>
       </c>
       <c r="BI25" s="4">
         <f t="shared" ref="BI25:BI36" si="44">E25-$I$19*BD25</f>
-        <v>0.29398324988004876</v>
+        <v>0.29429469640148009</v>
       </c>
     </row>
     <row r="26" spans="2:61">
       <c r="B26" s="19">
-        <f t="shared" si="29"/>
-        <v>0.14839653840986886</v>
+        <f t="shared" si="27"/>
+        <v>0.14840218546468847</v>
       </c>
       <c r="C26" s="19">
-        <f t="shared" si="29"/>
-        <v>0.1969916249400244</v>
+        <f t="shared" si="27"/>
+        <v>0.19714734820074004</v>
       </c>
       <c r="D26" s="19">
-        <f t="shared" si="29"/>
-        <v>0.24679307681973769</v>
+        <f t="shared" si="27"/>
+        <v>0.24680437092937696</v>
       </c>
       <c r="E26" s="19">
-        <f t="shared" si="29"/>
-        <v>0.29398324988004876</v>
+        <f t="shared" si="27"/>
+        <v>0.29429469640148009</v>
       </c>
       <c r="F26" s="20">
         <f t="shared" ref="F26:F36" si="45">F25</f>
         <v>0.3</v>
       </c>
       <c r="G26" s="21">
-        <f t="shared" si="30"/>
-        <v>0.33209913460246721</v>
+        <f t="shared" si="28"/>
+        <v>0.33210054636617209</v>
       </c>
       <c r="H26" s="21">
         <f t="shared" si="0"/>
-        <v>0.33924790623500611</v>
+        <v>0.33928683705018503</v>
       </c>
       <c r="I26" s="19">
-        <f t="shared" si="31"/>
-        <v>4.749662859255091E-2</v>
+        <f t="shared" si="29"/>
+        <v>4.8000088018557152E-2</v>
       </c>
       <c r="J26" s="19">
-        <f t="shared" si="31"/>
-        <v>0.65384437516256644</v>
+        <f t="shared" si="29"/>
+        <v>0.6496708787662655</v>
       </c>
       <c r="K26" s="19">
-        <f t="shared" si="31"/>
-        <v>0.14749662859254828</v>
+        <f t="shared" si="29"/>
+        <v>0.14014039228820011</v>
       </c>
       <c r="L26" s="19">
-        <f t="shared" si="31"/>
-        <v>0.78384437516256922</v>
+        <f t="shared" si="29"/>
+        <v>0.78412908651940816</v>
       </c>
       <c r="M26" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N26" s="21">
         <f t="shared" si="1"/>
-        <v>0.36581151167886528</v>
+        <v>0.36348864589902274</v>
       </c>
       <c r="O26" s="21">
         <f t="shared" si="2"/>
-        <v>0.7830587142441674</v>
+        <v>0.78180073140068873</v>
       </c>
       <c r="P26" s="22">
         <f t="shared" si="3"/>
-        <v>0.12660183184319929</v>
+        <v>0.12495422277952468</v>
       </c>
       <c r="Q26" s="22">
         <f t="shared" si="4"/>
-        <v>4.2824695750277163E-2</v>
+        <v>4.3346935445288157E-2</v>
       </c>
       <c r="R26" s="22">
         <f t="shared" si="5"/>
-        <v>0.16942652759347646</v>
+        <v>0.16830115822481284</v>
       </c>
       <c r="T26">
         <f t="shared" si="6"/>
-        <v>0.17664275782705374</v>
+        <v>0.17547093114279327</v>
       </c>
       <c r="U26">
         <f t="shared" si="7"/>
-        <v>0.72162302335772865</v>
+        <v>0.71697729179804326</v>
       </c>
       <c r="V26">
         <f t="shared" si="8"/>
-        <v>0.1653877018783598</v>
+        <v>0.1642371728528266</v>
       </c>
       <c r="W26">
         <f t="shared" si="9"/>
-        <v>-0.40388257151166562</v>
+        <v>-0.40639853719862395</v>
       </c>
       <c r="Y26">
         <f t="shared" si="10"/>
-        <v>0.36913250302488998</v>
+        <v>0.36680965136268445</v>
       </c>
       <c r="Z26">
+        <f t="shared" si="31"/>
+        <v>0.33210054636617081</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="32"/>
+        <v>0.33928683705018448</v>
+      </c>
+      <c r="AB26">
         <f t="shared" si="33"/>
-        <v>0.33209913460247042</v>
-      </c>
-      <c r="AA26">
+        <v>0.33210054636618747</v>
+      </c>
+      <c r="AC26">
         <f t="shared" si="34"/>
-        <v>0.33924790623500733</v>
-      </c>
-      <c r="AB26">
-        <f t="shared" si="35"/>
-        <v>0.33209913460248153</v>
-      </c>
-      <c r="AC26">
-        <f t="shared" si="36"/>
-        <v>0.33924790623500733</v>
+        <v>0.33928683705020113</v>
       </c>
       <c r="AE26">
         <f t="shared" si="11"/>
-        <v>0.23965038156631999</v>
+        <v>0.23810855033826764</v>
       </c>
       <c r="AF26">
+        <f t="shared" si="35"/>
+        <v>-0.13496517624608237</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" si="36"/>
+        <v>0.24326095757096527</v>
+      </c>
+      <c r="AH26">
         <f t="shared" si="12"/>
-        <v>-0.1370163167501432</v>
-      </c>
-      <c r="AG26">
-        <f t="shared" si="13"/>
-        <v>0.23965038156632801</v>
-      </c>
-      <c r="AH26">
-        <f t="shared" si="14"/>
-        <v>-0.1370163167501432</v>
+        <v>-0.13788567426794962</v>
       </c>
       <c r="AJ26">
         <f t="shared" si="37"/>
-        <v>-7.2328562190609083E-2</v>
+        <v>-7.1054187150576667E-2</v>
       </c>
       <c r="AK26">
         <f t="shared" si="38"/>
-        <v>0.72235253353763806</v>
+        <v>0.7171534668893067</v>
       </c>
       <c r="AL26">
         <f t="shared" si="39"/>
-        <v>2.7671437809384275E-2</v>
+        <v>1.8509913502717468E-2</v>
       </c>
       <c r="AM26">
         <f t="shared" si="40"/>
-        <v>0.85235253353764084</v>
+        <v>0.85307192365338302</v>
       </c>
       <c r="AO26">
+        <f t="shared" si="13"/>
+        <v>3.4414973113612808E-2</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="14"/>
+        <v>-0.26402529479115489</v>
+      </c>
+      <c r="AQ26">
         <f t="shared" si="15"/>
-        <v>3.427466072425573E-2</v>
-      </c>
-      <c r="AP26">
+        <v>-0.22961032167754208</v>
+      </c>
+      <c r="AR26">
         <f t="shared" si="16"/>
-        <v>-0.26407634760909554</v>
-      </c>
-      <c r="AQ26">
+        <v>0.1004774789343091</v>
+      </c>
+      <c r="AS26">
         <f t="shared" si="17"/>
-        <v>-0.22980168688483982</v>
-      </c>
-      <c r="AR26">
+        <v>-0.31866891373638073</v>
+      </c>
+      <c r="AT26">
         <f t="shared" si="18"/>
-        <v>0.1064369630600267</v>
-      </c>
-      <c r="AS26">
+        <v>-0.21819143480207165</v>
+      </c>
+      <c r="AV26">
         <f t="shared" si="19"/>
-        <v>-0.31658108190561324</v>
-      </c>
-      <c r="AT26">
+        <v>0.05</v>
+      </c>
+      <c r="AW26">
         <f t="shared" si="20"/>
-        <v>-0.21014411884558654</v>
-      </c>
-      <c r="AV26">
+        <v>0.1</v>
+      </c>
+      <c r="AX26">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW26">
+      <c r="AY26">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX26">
+      <c r="BA26" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY26">
+        <v>-1.1480516083877105E-2</v>
+      </c>
+      <c r="BB26" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA26" s="4">
+        <v>-1.0909571740103582E-2</v>
+      </c>
+      <c r="BC26" s="4">
         <f t="shared" si="25"/>
-        <v>-1.1490084344241992E-2</v>
-      </c>
-      <c r="BB26" s="4">
+        <v>-2.2961032167754209E-2</v>
+      </c>
+      <c r="BD26" s="4">
         <f t="shared" si="26"/>
-        <v>-1.0507205942279328E-2</v>
-      </c>
-      <c r="BC26" s="4">
-        <f t="shared" si="27"/>
-        <v>-2.2980168688483984E-2</v>
-      </c>
-      <c r="BD26" s="4">
-        <f t="shared" si="28"/>
-        <v>-2.1014411884558656E-2</v>
+        <v>-2.1819143480207165E-2</v>
       </c>
       <c r="BE26" s="4"/>
       <c r="BF26" s="4">
         <f t="shared" si="41"/>
-        <v>0.15414158058198985</v>
+        <v>0.15414244350662704</v>
       </c>
       <c r="BG26" s="4">
         <f t="shared" si="42"/>
-        <v>0.20224522791116406</v>
+        <v>0.20260213407079183</v>
       </c>
       <c r="BH26" s="4">
         <f t="shared" si="43"/>
-        <v>0.2582831611639797</v>
+        <v>0.25828488701325408</v>
       </c>
       <c r="BI26" s="4">
         <f t="shared" si="44"/>
-        <v>0.30449045582232809</v>
+        <v>0.30520426814158369</v>
       </c>
     </row>
     <row r="27" spans="2:61">
       <c r="B27" s="19">
-        <f t="shared" si="29"/>
-        <v>0.15414158058198985</v>
+        <f t="shared" si="27"/>
+        <v>0.15414244350662704</v>
       </c>
       <c r="C27" s="19">
-        <f t="shared" si="29"/>
-        <v>0.20224522791116406</v>
+        <f t="shared" si="27"/>
+        <v>0.20260213407079183</v>
       </c>
       <c r="D27" s="19">
-        <f t="shared" si="29"/>
-        <v>0.2582831611639797</v>
+        <f t="shared" si="27"/>
+        <v>0.25828488701325408</v>
       </c>
       <c r="E27" s="19">
-        <f t="shared" si="29"/>
-        <v>0.30449045582232809</v>
+        <f t="shared" si="27"/>
+        <v>0.30520426814158369</v>
       </c>
       <c r="F27" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G27" s="21">
-        <f t="shared" si="30"/>
-        <v>0.33353539514549746</v>
+        <f t="shared" si="28"/>
+        <v>0.33353561087665673</v>
       </c>
       <c r="H27" s="21">
         <f t="shared" si="0"/>
-        <v>0.34056130697779102</v>
+        <v>0.34065053351769797</v>
       </c>
       <c r="I27" s="19">
-        <f t="shared" si="31"/>
-        <v>-7.2328562190609083E-2</v>
+        <f t="shared" si="29"/>
+        <v>-7.1054187150576667E-2</v>
       </c>
       <c r="J27" s="19">
-        <f t="shared" si="31"/>
-        <v>0.72235253353763806</v>
+        <f t="shared" si="29"/>
+        <v>0.7171534668893067</v>
       </c>
       <c r="K27" s="19">
-        <f t="shared" si="31"/>
-        <v>2.7671437809384275E-2</v>
+        <f t="shared" si="29"/>
+        <v>1.8509913502717468E-2</v>
       </c>
       <c r="L27" s="19">
-        <f t="shared" si="31"/>
-        <v>0.85235253353764084</v>
+        <f t="shared" si="29"/>
+        <v>0.85307192365338302</v>
       </c>
       <c r="M27" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N27" s="21">
         <f t="shared" si="1"/>
-        <v>0.28529968545576806</v>
+        <v>0.28260631019345528</v>
       </c>
       <c r="O27" s="21">
         <f t="shared" si="2"/>
-        <v>0.83120843053523763</v>
+        <v>0.82979562559273101</v>
       </c>
       <c r="P27" s="22">
         <f t="shared" si="3"/>
-        <v>7.5789916812044833E-2</v>
+        <v>7.4314200357290361E-2</v>
       </c>
       <c r="Q27" s="22">
         <f t="shared" si="4"/>
-        <v>2.5214762533082451E-2</v>
+        <v>2.5665441579224419E-2</v>
       </c>
       <c r="R27" s="22">
         <f t="shared" si="5"/>
-        <v>0.10100467934512729</v>
+        <v>9.9979641936514776E-2</v>
       </c>
       <c r="T27">
         <f t="shared" si="6"/>
-        <v>0.10661067305424264</v>
+        <v>0.10553176814038388</v>
       </c>
       <c r="U27">
         <f t="shared" si="7"/>
-        <v>0.56059937091153533</v>
+        <v>0.55521262038691066</v>
       </c>
       <c r="V27">
         <f t="shared" si="8"/>
-        <v>9.7928847955832038E-2</v>
+        <v>9.68755544483694E-2</v>
       </c>
       <c r="W27">
         <f t="shared" si="9"/>
-        <v>-0.30758313892952499</v>
+        <v>-0.31040874881453767</v>
       </c>
       <c r="Y27">
         <f t="shared" si="10"/>
-        <v>0.28863503940722307</v>
+        <v>0.28594166630222184</v>
       </c>
       <c r="Z27">
+        <f t="shared" si="31"/>
+        <v>0.33353561087665629</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="32"/>
+        <v>0.34065053351769459</v>
+      </c>
+      <c r="AB27">
         <f t="shared" si="33"/>
-        <v>0.33353539514550112</v>
-      </c>
-      <c r="AA27">
+        <v>0.33353561087665629</v>
+      </c>
+      <c r="AC27">
         <f t="shared" si="34"/>
-        <v>0.34056130697779352</v>
-      </c>
-      <c r="AB27">
-        <f t="shared" si="35"/>
-        <v>0.33353539514551223</v>
-      </c>
-      <c r="AC27">
-        <f t="shared" si="36"/>
-        <v>0.34056130697779352</v>
+        <v>0.34065053351768348</v>
       </c>
       <c r="AE27">
         <f t="shared" si="11"/>
-        <v>0.18697973269529827</v>
+        <v>0.1851831805071773</v>
       </c>
       <c r="AF27">
+        <f t="shared" si="35"/>
+        <v>-0.10353237165731538</v>
+      </c>
+      <c r="AG27">
+        <f t="shared" si="36"/>
+        <v>0.18913347535055836</v>
+      </c>
+      <c r="AH27">
         <f t="shared" si="12"/>
-        <v>-0.10475091579817128</v>
-      </c>
-      <c r="AG27">
-        <f t="shared" si="13"/>
-        <v>0.18697973269530452</v>
-      </c>
-      <c r="AH27">
-        <f t="shared" si="14"/>
-        <v>-0.10475091579817128</v>
+        <v>-0.10574090589222886</v>
       </c>
       <c r="AJ27">
         <f t="shared" si="37"/>
-        <v>-0.16581842853825823</v>
+        <v>-0.1636457774041653</v>
       </c>
       <c r="AK27">
         <f t="shared" si="38"/>
-        <v>0.77472799143672366</v>
+        <v>0.76891965271796436</v>
       </c>
       <c r="AL27">
         <f t="shared" si="39"/>
-        <v>-6.5818428538267984E-2</v>
+        <v>-7.605682417256171E-2</v>
       </c>
       <c r="AM27">
         <f t="shared" si="40"/>
-        <v>0.90472799143672644</v>
+        <v>0.9059423765994975</v>
       </c>
       <c r="AO27">
+        <f t="shared" si="13"/>
+        <v>-3.9450181437333628E-2</v>
+      </c>
+      <c r="AP27">
+        <f t="shared" si="14"/>
+        <v>-0.22261071036511768</v>
+      </c>
+      <c r="AQ27">
         <f t="shared" si="15"/>
-        <v>-4.054734646299131E-2</v>
-      </c>
-      <c r="AP27">
+        <v>-0.26206089180245129</v>
+      </c>
+      <c r="AR27">
         <f t="shared" si="16"/>
-        <v>-0.22218345967920169</v>
-      </c>
-      <c r="AQ27">
+        <v>1.0276937578978825E-2</v>
+      </c>
+      <c r="AS27">
         <f t="shared" si="17"/>
-        <v>-0.26273080614219302</v>
-      </c>
-      <c r="AR27">
+        <v>-0.26480098847005745</v>
+      </c>
+      <c r="AT27">
         <f t="shared" si="18"/>
-        <v>1.5512590628158497E-2</v>
-      </c>
-      <c r="AS27">
+        <v>-0.2545240508910786</v>
+      </c>
+      <c r="AV27">
         <f t="shared" si="19"/>
-        <v>-0.26216926774004079</v>
-      </c>
-      <c r="AT27">
+        <v>0.05</v>
+      </c>
+      <c r="AW27">
         <f t="shared" si="20"/>
-        <v>-0.2466566771118823</v>
-      </c>
-      <c r="AV27">
+        <v>0.1</v>
+      </c>
+      <c r="AX27">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW27">
+      <c r="AY27">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX27">
+      <c r="BA27" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY27">
+        <v>-1.3103044590122565E-2</v>
+      </c>
+      <c r="BB27" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA27" s="4">
+        <v>-1.272620254455393E-2</v>
+      </c>
+      <c r="BC27" s="4">
         <f t="shared" si="25"/>
-        <v>-1.3136540307109652E-2</v>
-      </c>
-      <c r="BB27" s="4">
+        <v>-2.620608918024513E-2</v>
+      </c>
+      <c r="BD27" s="4">
         <f t="shared" si="26"/>
-        <v>-1.2332833855594116E-2</v>
-      </c>
-      <c r="BC27" s="4">
-        <f t="shared" si="27"/>
-        <v>-2.6273080614219305E-2</v>
-      </c>
-      <c r="BD27" s="4">
-        <f t="shared" si="28"/>
-        <v>-2.4665667711188232E-2</v>
+        <v>-2.5452405089107861E-2</v>
       </c>
       <c r="BE27" s="4"/>
       <c r="BF27" s="4">
         <f t="shared" si="41"/>
-        <v>0.16070985073554467</v>
+        <v>0.16069396580168832</v>
       </c>
       <c r="BG27" s="4">
         <f t="shared" si="42"/>
-        <v>0.20841164483896113</v>
+        <v>0.20896523534306879</v>
       </c>
       <c r="BH27" s="4">
         <f t="shared" si="43"/>
-        <v>0.27141970147108935</v>
+        <v>0.27138793160337665</v>
       </c>
       <c r="BI27" s="4">
         <f t="shared" si="44"/>
-        <v>0.31682328967792223</v>
+        <v>0.31793047068613761</v>
       </c>
     </row>
     <row r="28" spans="2:61">
       <c r="B28" s="19">
-        <f t="shared" si="29"/>
-        <v>0.16070985073554467</v>
+        <f t="shared" si="27"/>
+        <v>0.16069396580168832</v>
       </c>
       <c r="C28" s="19">
-        <f t="shared" si="29"/>
-        <v>0.20841164483896113</v>
+        <f t="shared" si="27"/>
+        <v>0.20896523534306879</v>
       </c>
       <c r="D28" s="19">
-        <f t="shared" si="29"/>
-        <v>0.27141970147108935</v>
+        <f t="shared" si="27"/>
+        <v>0.27138793160337665</v>
       </c>
       <c r="E28" s="19">
-        <f t="shared" si="29"/>
-        <v>0.31682328967792223</v>
+        <f t="shared" si="27"/>
+        <v>0.31793047068613761</v>
       </c>
       <c r="F28" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G28" s="21">
-        <f t="shared" si="30"/>
-        <v>0.33517746268388615</v>
+        <f t="shared" si="28"/>
+        <v>0.33517349145042208</v>
       </c>
       <c r="H28" s="21">
         <f t="shared" si="0"/>
-        <v>0.34210291120974029</v>
+        <v>0.3422413088357672</v>
       </c>
       <c r="I28" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.16581842853825823</v>
+        <f t="shared" si="29"/>
+        <v>-0.1636457774041653</v>
       </c>
       <c r="J28" s="19">
-        <f t="shared" si="31"/>
-        <v>0.77472799143672366</v>
+        <f t="shared" si="29"/>
+        <v>0.76891965271796436</v>
       </c>
       <c r="K28" s="19">
-        <f t="shared" si="31"/>
-        <v>-6.5818428538267984E-2</v>
+        <f t="shared" si="29"/>
+        <v>-7.605682417256171E-2</v>
       </c>
       <c r="L28" s="19">
-        <f t="shared" si="31"/>
-        <v>0.90472799143672644</v>
+        <f t="shared" si="29"/>
+        <v>0.9059423765994975</v>
       </c>
       <c r="M28" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N28" s="21">
         <f t="shared" si="1"/>
-        <v>0.22190472384212556</v>
+        <v>0.21912048637561798</v>
       </c>
       <c r="O28" s="21">
         <f t="shared" si="2"/>
-        <v>0.86918144216338966</v>
+        <v>0.86777238934352363</v>
       </c>
       <c r="P28" s="22">
         <f t="shared" si="3"/>
-        <v>4.4903611986607493E-2</v>
+        <v>4.3731377821975025E-2</v>
       </c>
       <c r="Q28" s="22">
         <f t="shared" si="4"/>
-        <v>1.4597123917718354E-2</v>
+        <v>1.4939588806791174E-2</v>
       </c>
       <c r="R28" s="22">
         <f t="shared" si="5"/>
-        <v>5.9500735904325849E-2</v>
+        <v>5.8670966628766197E-2</v>
       </c>
       <c r="T28">
         <f t="shared" si="6"/>
-        <v>6.383883038116836E-2</v>
+        <v>6.2953376356278568E-2</v>
       </c>
       <c r="U28">
         <f t="shared" si="7"/>
-        <v>0.43380944768425106</v>
+        <v>0.42824097275123707</v>
       </c>
       <c r="V28">
         <f t="shared" si="8"/>
-        <v>5.7184364747593641E-2</v>
+        <v>5.6326414415636669E-2</v>
       </c>
       <c r="W28">
         <f t="shared" si="9"/>
-        <v>-0.23163711567322082</v>
+        <v>-0.23445522131295277</v>
       </c>
       <c r="Y28">
         <f t="shared" si="10"/>
-        <v>0.22525649846896445</v>
+        <v>0.2224722212901222</v>
       </c>
       <c r="Z28">
+        <f t="shared" si="31"/>
+        <v>0.33517349145042175</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="32"/>
+        <v>0.34224130883576676</v>
+      </c>
+      <c r="AB28">
         <f t="shared" si="33"/>
-        <v>0.33517746268388882</v>
-      </c>
-      <c r="AA28">
+        <v>0.33517349145042452</v>
+      </c>
+      <c r="AC28">
         <f t="shared" si="34"/>
-        <v>0.34210291120974068</v>
-      </c>
-      <c r="AB28">
-        <f t="shared" si="35"/>
-        <v>0.33517746268387771</v>
-      </c>
-      <c r="AC28">
-        <f t="shared" si="36"/>
-        <v>0.34210291120972958</v>
+        <v>0.34224130883577786</v>
       </c>
       <c r="AE28">
         <f t="shared" si="11"/>
-        <v>0.14540314996310647</v>
+        <v>0.14353502201915705</v>
       </c>
       <c r="AF28">
+        <f t="shared" si="35"/>
+        <v>-7.8583175116244366E-2</v>
+      </c>
+      <c r="AG28">
+        <f t="shared" si="36"/>
+        <v>0.1465617510114853</v>
+      </c>
+      <c r="AH28">
         <f t="shared" si="12"/>
-        <v>-7.9243731616036289E-2</v>
-      </c>
-      <c r="AG28">
-        <f t="shared" si="13"/>
-        <v>0.14540314996310166</v>
-      </c>
-      <c r="AH28">
-        <f t="shared" si="14"/>
-        <v>-7.9243731616033722E-2</v>
+        <v>-8.0240261805526916E-2</v>
       </c>
       <c r="AJ28">
         <f t="shared" si="37"/>
-        <v>-0.23852000351981145</v>
+        <v>-0.23541328841374382</v>
       </c>
       <c r="AK28">
         <f t="shared" si="38"/>
-        <v>0.81434985724474185</v>
+        <v>0.8082112402760866</v>
       </c>
       <c r="AL28">
         <f t="shared" si="39"/>
-        <v>-0.1385200035198188</v>
+        <v>-0.14933769967830435</v>
       </c>
       <c r="AM28">
         <f t="shared" si="40"/>
-        <v>0.9443498572447433</v>
+        <v>0.94606250750226095</v>
       </c>
       <c r="AO28">
+        <f t="shared" si="13"/>
+        <v>-7.0079826902192166E-2</v>
+      </c>
+      <c r="AP28">
+        <f t="shared" si="14"/>
+        <v>-0.18027722734986912</v>
+      </c>
+      <c r="AQ28">
         <f t="shared" si="15"/>
-        <v>-7.1933600900052255E-2</v>
-      </c>
-      <c r="AP28">
+        <v>-0.25035705425206128</v>
+      </c>
+      <c r="AR28">
         <f t="shared" si="16"/>
-        <v>-0.17945575736771038</v>
-      </c>
-      <c r="AQ28">
+        <v>-3.257064836802763E-2</v>
+      </c>
+      <c r="AS28">
         <f t="shared" si="17"/>
-        <v>-0.25138935826776265</v>
-      </c>
-      <c r="AR28">
+        <v>-0.21240292040241759</v>
+      </c>
+      <c r="AT28">
         <f t="shared" si="18"/>
-        <v>-2.8552656131631382E-2</v>
-      </c>
-      <c r="AS28">
+        <v>-0.24497356877044524</v>
+      </c>
+      <c r="AV28">
         <f t="shared" si="19"/>
-        <v>-0.20956858240522974</v>
-      </c>
-      <c r="AT28">
+        <v>0.05</v>
+      </c>
+      <c r="AW28">
         <f t="shared" si="20"/>
-        <v>-0.23812123853686112</v>
-      </c>
-      <c r="AV28">
+        <v>0.1</v>
+      </c>
+      <c r="AX28">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW28">
+      <c r="AY28">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX28">
+      <c r="BA28" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY28">
+        <v>-1.2517852712603065E-2</v>
+      </c>
+      <c r="BB28" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA28" s="4">
+        <v>-1.2248678438522263E-2</v>
+      </c>
+      <c r="BC28" s="4">
         <f t="shared" si="25"/>
-        <v>-1.2569467913388133E-2</v>
-      </c>
-      <c r="BB28" s="4">
+        <v>-2.5035705425206129E-2</v>
+      </c>
+      <c r="BD28" s="4">
         <f t="shared" si="26"/>
-        <v>-1.1906061926843056E-2</v>
-      </c>
-      <c r="BC28" s="4">
-        <f t="shared" si="27"/>
-        <v>-2.5138935826776267E-2</v>
-      </c>
-      <c r="BD28" s="4">
-        <f t="shared" si="28"/>
-        <v>-2.3812123853686112E-2</v>
+        <v>-2.4497356877044525E-2</v>
       </c>
       <c r="BE28" s="4"/>
       <c r="BF28" s="4">
         <f t="shared" si="41"/>
-        <v>0.16699458469223874</v>
+        <v>0.16695289215798986</v>
       </c>
       <c r="BG28" s="4">
         <f t="shared" si="42"/>
-        <v>0.21436467580238266</v>
+        <v>0.21508957456232994</v>
       </c>
       <c r="BH28" s="4">
         <f t="shared" si="43"/>
-        <v>0.28398916938447749</v>
+        <v>0.28390578431597974</v>
       </c>
       <c r="BI28" s="4">
         <f t="shared" si="44"/>
-        <v>0.3287293516047653</v>
+        <v>0.3301791491246599</v>
       </c>
     </row>
     <row r="29" spans="2:61">
       <c r="B29" s="19">
-        <f t="shared" si="29"/>
-        <v>0.16699458469223874</v>
+        <f t="shared" si="27"/>
+        <v>0.16695289215798986</v>
       </c>
       <c r="C29" s="19">
-        <f t="shared" si="29"/>
-        <v>0.21436467580238266</v>
+        <f t="shared" si="27"/>
+        <v>0.21508957456232994</v>
       </c>
       <c r="D29" s="19">
-        <f t="shared" si="29"/>
-        <v>0.28398916938447749</v>
+        <f t="shared" si="27"/>
+        <v>0.28390578431597974</v>
       </c>
       <c r="E29" s="19">
-        <f t="shared" si="29"/>
-        <v>0.3287293516047653</v>
+        <f t="shared" si="27"/>
+        <v>0.3301791491246599</v>
       </c>
       <c r="F29" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G29" s="21">
-        <f t="shared" si="30"/>
-        <v>0.33674864617305966</v>
+        <f t="shared" si="28"/>
+        <v>0.33673822303949746</v>
       </c>
       <c r="H29" s="21">
         <f t="shared" si="0"/>
-        <v>0.34359116895059566</v>
+        <v>0.34377239364058249</v>
       </c>
       <c r="I29" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.23852000351981145</v>
+        <f t="shared" si="29"/>
+        <v>-0.23541328841374382</v>
       </c>
       <c r="J29" s="19">
-        <f t="shared" si="31"/>
-        <v>0.81434985724474185</v>
+        <f t="shared" si="29"/>
+        <v>0.8082112402760866</v>
       </c>
       <c r="K29" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.1385200035198188</v>
+        <f t="shared" si="29"/>
+        <v>-0.14933769967830435</v>
       </c>
       <c r="L29" s="19">
-        <f t="shared" si="31"/>
-        <v>0.9443498572447433</v>
+        <f t="shared" si="29"/>
+        <v>0.94606250750226095</v>
       </c>
       <c r="M29" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N29" s="21">
         <f t="shared" si="1"/>
-        <v>0.17208446179709491</v>
+        <v>0.16938916910048205</v>
       </c>
       <c r="O29" s="21">
         <f t="shared" si="2"/>
-        <v>0.89870148328744071</v>
+        <v>0.89738578962878157</v>
       </c>
       <c r="P29" s="22">
         <f t="shared" si="3"/>
-        <v>2.6271372756053919E-2</v>
+        <v>2.5404907226542057E-2</v>
       </c>
       <c r="Q29" s="22">
         <f t="shared" si="4"/>
-        <v>8.3354191539134672E-3</v>
+        <v>8.5773919626843022E-3</v>
       </c>
       <c r="R29" s="22">
         <f t="shared" si="5"/>
-        <v>3.4606791909967384E-2</v>
+        <v>3.3982299189226357E-2</v>
       </c>
       <c r="T29">
         <f t="shared" si="6"/>
-        <v>3.7948481145909284E-2</v>
+        <v>3.7270082571236006E-2</v>
       </c>
       <c r="U29">
         <f t="shared" si="7"/>
-        <v>0.33416892359418998</v>
+        <v>0.32877833820096486</v>
       </c>
       <c r="V29">
         <f t="shared" si="8"/>
-        <v>3.2880821575716201E-2</v>
+        <v>3.2230014981801988E-2</v>
       </c>
       <c r="W29">
         <f t="shared" si="9"/>
-        <v>-0.17259703342511826</v>
+        <v>-0.17522842074243691</v>
       </c>
       <c r="Y29">
         <f t="shared" si="10"/>
-        <v>0.17545194825882549</v>
+        <v>0.17275655133087703</v>
       </c>
       <c r="Z29">
+        <f t="shared" si="31"/>
+        <v>0.3367382230394983</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="32"/>
+        <v>0.34377239364058176</v>
+      </c>
+      <c r="AB29">
         <f t="shared" si="33"/>
-        <v>0.33674864617305733</v>
-      </c>
-      <c r="AA29">
+        <v>0.33673822303947887</v>
+      </c>
+      <c r="AC29">
         <f t="shared" si="34"/>
-        <v>0.34359116895059383</v>
-      </c>
-      <c r="AB29">
-        <f t="shared" si="35"/>
-        <v>0.33674864617305733</v>
-      </c>
-      <c r="AC29">
-        <f t="shared" si="36"/>
-        <v>0.3435911689505966</v>
+        <v>0.34377239364058454</v>
       </c>
       <c r="AE29">
         <f t="shared" si="11"/>
-        <v>0.11253093261345132</v>
+        <v>0.11071223337967211</v>
       </c>
       <c r="AF29">
+        <f t="shared" si="35"/>
+        <v>-5.9006107026822366E-2</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" si="36"/>
+        <v>0.11302491630051842</v>
+      </c>
+      <c r="AH29">
         <f t="shared" si="12"/>
-        <v>-5.9302816471941099E-2</v>
-      </c>
-      <c r="AG29">
-        <f t="shared" si="13"/>
-        <v>0.11253093261345132</v>
-      </c>
-      <c r="AH29">
-        <f t="shared" si="14"/>
-        <v>-5.9302816471941577E-2</v>
+        <v>-6.0238693632486989E-2</v>
       </c>
       <c r="AJ29">
         <f t="shared" si="37"/>
-        <v>-0.29478546982653708</v>
+        <v>-0.29076940510357985</v>
       </c>
       <c r="AK29">
         <f t="shared" si="38"/>
-        <v>0.84400126548071241</v>
+        <v>0.8377142937894978</v>
       </c>
       <c r="AL29">
         <f t="shared" si="39"/>
-        <v>-0.19478546982654446</v>
+        <v>-0.20585015782856356</v>
       </c>
       <c r="AM29">
         <f t="shared" si="40"/>
-        <v>0.97400126548071408</v>
+        <v>0.97618185431850446</v>
       </c>
       <c r="AO29">
+        <f t="shared" si="13"/>
+        <v>-7.7398789755095149E-2</v>
+      </c>
+      <c r="AP29">
+        <f t="shared" si="14"/>
+        <v>-0.14162157925986488</v>
+      </c>
+      <c r="AQ29">
         <f t="shared" si="15"/>
-        <v>-7.9705972831897801E-2</v>
-      </c>
-      <c r="AP29">
+        <v>-0.21902036901496003</v>
+      </c>
+      <c r="AR29">
         <f t="shared" si="16"/>
-        <v>-0.14055436953061098</v>
-      </c>
-      <c r="AQ29">
+        <v>-4.909900073098767E-2</v>
+      </c>
+      <c r="AS29">
         <f t="shared" si="17"/>
-        <v>-0.2202603423625088</v>
-      </c>
-      <c r="AR29">
+        <v>-0.16577703911325106</v>
+      </c>
+      <c r="AT29">
         <f t="shared" si="18"/>
-        <v>-4.6289080472481259E-2</v>
-      </c>
-      <c r="AS29">
+        <v>-0.21487603984423873</v>
+      </c>
+      <c r="AV29">
         <f t="shared" si="19"/>
-        <v>-0.1629919838758766</v>
-      </c>
-      <c r="AT29">
+        <v>0.05</v>
+      </c>
+      <c r="AW29">
         <f t="shared" si="20"/>
-        <v>-0.20928106434835786</v>
-      </c>
-      <c r="AV29">
+        <v>0.1</v>
+      </c>
+      <c r="AX29">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW29">
+      <c r="AY29">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX29">
+      <c r="BA29" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY29">
+        <v>-1.0951018450748001E-2</v>
+      </c>
+      <c r="BB29" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA29" s="4">
+        <v>-1.0743801992211937E-2</v>
+      </c>
+      <c r="BC29" s="4">
         <f t="shared" si="25"/>
-        <v>-1.101301711812544E-2</v>
-      </c>
-      <c r="BB29" s="4">
+        <v>-2.1902036901496003E-2</v>
+      </c>
+      <c r="BD29" s="4">
         <f t="shared" si="26"/>
-        <v>-1.0464053217417894E-2</v>
-      </c>
-      <c r="BC29" s="4">
-        <f t="shared" si="27"/>
-        <v>-2.202603423625088E-2</v>
-      </c>
-      <c r="BD29" s="4">
-        <f t="shared" si="28"/>
-        <v>-2.0928106434835787E-2</v>
+        <v>-2.1487603984423873E-2</v>
       </c>
       <c r="BE29" s="4"/>
       <c r="BF29" s="4">
         <f t="shared" si="41"/>
-        <v>0.17250109325130147</v>
+        <v>0.17242840138336385</v>
       </c>
       <c r="BG29" s="4">
         <f t="shared" si="42"/>
-        <v>0.21959670241109161</v>
+        <v>0.2204614755584359</v>
       </c>
       <c r="BH29" s="4">
         <f t="shared" si="43"/>
-        <v>0.2950021865026029</v>
+        <v>0.29485680276672777</v>
       </c>
       <c r="BI29" s="4">
         <f t="shared" si="44"/>
-        <v>0.33919340482218319</v>
+        <v>0.34092295111687182</v>
       </c>
     </row>
     <row r="30" spans="2:61">
       <c r="B30" s="19">
-        <f t="shared" si="29"/>
-        <v>0.17250109325130147</v>
+        <f t="shared" si="27"/>
+        <v>0.17242840138336385</v>
       </c>
       <c r="C30" s="19">
-        <f t="shared" si="29"/>
-        <v>0.21959670241109161</v>
+        <f t="shared" si="27"/>
+        <v>0.2204614755584359</v>
       </c>
       <c r="D30" s="19">
-        <f t="shared" si="29"/>
-        <v>0.2950021865026029</v>
+        <f t="shared" si="27"/>
+        <v>0.29485680276672777</v>
       </c>
       <c r="E30" s="19">
-        <f t="shared" si="29"/>
-        <v>0.33919340482218319</v>
+        <f t="shared" si="27"/>
+        <v>0.34092295111687182</v>
       </c>
       <c r="F30" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G30" s="21">
-        <f t="shared" si="30"/>
-        <v>0.33812527331282538</v>
+        <f t="shared" si="28"/>
+        <v>0.33810710034584096</v>
       </c>
       <c r="H30" s="21">
         <f t="shared" si="0"/>
-        <v>0.34489917560277289</v>
+        <v>0.34511536888960898</v>
       </c>
       <c r="I30" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.29478546982653708</v>
+        <f t="shared" si="29"/>
+        <v>-0.29076940510357985</v>
       </c>
       <c r="J30" s="19">
-        <f t="shared" si="31"/>
-        <v>0.84400126548071241</v>
+        <f t="shared" si="29"/>
+        <v>0.8377142937894978</v>
       </c>
       <c r="K30" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.19478546982654446</v>
+        <f t="shared" si="29"/>
+        <v>-0.20585015782856356</v>
       </c>
       <c r="L30" s="19">
-        <f t="shared" si="31"/>
-        <v>0.97400126548071408</v>
+        <f t="shared" si="29"/>
+        <v>0.97618185431850446</v>
       </c>
       <c r="M30" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N30" s="21">
         <f t="shared" si="1"/>
-        <v>0.13314423448367851</v>
+        <v>0.13064674641615448</v>
       </c>
       <c r="O30" s="21">
         <f t="shared" si="2"/>
-        <v>0.92131039206739218</v>
+        <v>0.92013251154790421</v>
       </c>
       <c r="P30" s="22">
         <f t="shared" si="3"/>
-        <v>1.5164502486571198E-2</v>
+        <v>1.4555637420803885E-2</v>
       </c>
       <c r="Q30" s="22">
         <f t="shared" si="4"/>
-        <v>4.718262237935378E-3</v>
+        <v>4.8814659426037379E-3</v>
       </c>
       <c r="R30" s="22">
         <f t="shared" si="5"/>
-        <v>1.9882764724506577E-2</v>
+        <v>1.9437103363407621E-2</v>
       </c>
       <c r="T30">
         <f t="shared" si="6"/>
-        <v>2.2445649414180143E-2</v>
+        <v>2.1950038291730714E-2</v>
       </c>
       <c r="U30">
         <f t="shared" si="7"/>
-        <v>0.25628846896735663</v>
+        <v>0.25129349283230934</v>
       </c>
       <c r="V30">
         <f t="shared" si="8"/>
-        <v>1.860897256585442E-2</v>
+        <v>1.8139753594365704E-2</v>
       </c>
       <c r="W30">
         <f t="shared" si="9"/>
-        <v>-0.12737921586521567</v>
+        <v>-0.12973497690419167</v>
       </c>
       <c r="Y30">
         <f t="shared" si="10"/>
-        <v>0.13652548721680677</v>
+        <v>0.13402781741961289</v>
       </c>
       <c r="Z30">
+        <f t="shared" si="31"/>
+        <v>0.33810710034584135</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="32"/>
+        <v>0.34511536888960914</v>
+      </c>
+      <c r="AB30">
         <f t="shared" si="33"/>
-        <v>0.33812527331282538</v>
-      </c>
-      <c r="AA30">
+        <v>0.33810710034585245</v>
+      </c>
+      <c r="AC30">
         <f t="shared" si="34"/>
-        <v>0.34489917560277528</v>
-      </c>
-      <c r="AB30">
-        <f t="shared" si="35"/>
-        <v>0.33812527331282816</v>
-      </c>
-      <c r="AC30">
-        <f t="shared" si="36"/>
-        <v>0.34489917560276417</v>
+        <v>0.34511536888961469</v>
       </c>
       <c r="AE30">
         <f t="shared" si="11"/>
-        <v>8.6657608616513032E-2</v>
+        <v>8.4964114197310578E-2</v>
       </c>
       <c r="AF30">
+        <f t="shared" si="35"/>
+        <v>-4.3864316854512385E-2</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="36"/>
+        <v>8.6725246478380785E-2</v>
+      </c>
+      <c r="AH30">
         <f t="shared" si="12"/>
-        <v>-4.3932986540840838E-2</v>
-      </c>
-      <c r="AG30">
-        <f t="shared" si="13"/>
-        <v>8.665760861651374E-2</v>
-      </c>
-      <c r="AH30">
-        <f t="shared" si="14"/>
-        <v>-4.3932986540839422E-2</v>
+        <v>-4.4773534412175749E-2</v>
       </c>
       <c r="AJ30">
         <f t="shared" si="37"/>
-        <v>-0.33811427413479361</v>
+        <v>-0.33325146220223512</v>
       </c>
       <c r="AK30">
         <f t="shared" si="38"/>
-        <v>0.86596775875113285</v>
+        <v>0.85964645221675395</v>
       </c>
       <c r="AL30">
         <f t="shared" si="39"/>
-        <v>-0.23811427413480132</v>
+        <v>-0.24921278106775396</v>
       </c>
       <c r="AM30">
         <f t="shared" si="40"/>
-        <v>0.99596775875113375</v>
+        <v>0.99856862152459236</v>
       </c>
       <c r="AO30">
+        <f t="shared" si="13"/>
+        <v>-7.3068459417251291E-2</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" si="14"/>
+        <v>-0.10868084455709173</v>
+      </c>
+      <c r="AQ30">
         <f t="shared" si="15"/>
-        <v>-7.5550116735666098E-2</v>
-      </c>
-      <c r="AP30">
+        <v>-0.18174930397434302</v>
+      </c>
+      <c r="AR30">
         <f t="shared" si="16"/>
-        <v>-0.10750821938618287</v>
-      </c>
-      <c r="AQ30">
+        <v>-5.1728805160821879E-2</v>
+      </c>
+      <c r="AS30">
         <f t="shared" si="17"/>
-        <v>-0.18305833612184896</v>
-      </c>
-      <c r="AR30">
+        <v>-0.12664493032430219</v>
+      </c>
+      <c r="AT30">
         <f t="shared" si="18"/>
-        <v>-4.9921269838932324E-2</v>
-      </c>
-      <c r="AS30">
+        <v>-0.17837373548512406</v>
+      </c>
+      <c r="AV30">
         <f t="shared" si="19"/>
-        <v>-0.12406751744866111</v>
-      </c>
-      <c r="AT30">
+        <v>0.05</v>
+      </c>
+      <c r="AW30">
         <f t="shared" si="20"/>
-        <v>-0.17398878728759343</v>
-      </c>
-      <c r="AV30">
+        <v>0.1</v>
+      </c>
+      <c r="AX30">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW30">
+      <c r="AY30">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX30">
+      <c r="BA30" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY30">
+        <v>-9.0874651987171515E-3</v>
+      </c>
+      <c r="BB30" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA30" s="4">
+        <v>-8.9186867742562029E-3</v>
+      </c>
+      <c r="BC30" s="4">
         <f t="shared" si="25"/>
-        <v>-9.1529168060924485E-3</v>
-      </c>
-      <c r="BB30" s="4">
+        <v>-1.8174930397434303E-2</v>
+      </c>
+      <c r="BD30" s="4">
         <f t="shared" si="26"/>
-        <v>-8.6994393643796721E-3</v>
-      </c>
-      <c r="BC30" s="4">
-        <f t="shared" si="27"/>
-        <v>-1.8305833612184897E-2</v>
-      </c>
-      <c r="BD30" s="4">
-        <f t="shared" si="28"/>
-        <v>-1.7398878728759344E-2</v>
+        <v>-1.7837373548512406E-2</v>
       </c>
       <c r="BE30" s="4"/>
       <c r="BF30" s="4">
         <f t="shared" si="41"/>
-        <v>0.17707755165434769</v>
+        <v>0.17697213398272243</v>
       </c>
       <c r="BG30" s="4">
         <f t="shared" si="42"/>
-        <v>0.22394642209328144</v>
+        <v>0.22492081894556401</v>
       </c>
       <c r="BH30" s="4">
         <f t="shared" si="43"/>
-        <v>0.30415510330869533</v>
+        <v>0.30394426796544494</v>
       </c>
       <c r="BI30" s="4">
         <f t="shared" si="44"/>
-        <v>0.34789284418656286</v>
+        <v>0.34984163789112804</v>
       </c>
     </row>
     <row r="31" spans="2:61">
       <c r="B31" s="19">
-        <f t="shared" si="29"/>
-        <v>0.17707755165434769</v>
+        <f t="shared" si="27"/>
+        <v>0.17697213398272243</v>
       </c>
       <c r="C31" s="19">
-        <f t="shared" si="29"/>
-        <v>0.22394642209328144</v>
+        <f t="shared" si="27"/>
+        <v>0.22492081894556401</v>
       </c>
       <c r="D31" s="19">
-        <f t="shared" si="29"/>
-        <v>0.30415510330869533</v>
+        <f t="shared" si="27"/>
+        <v>0.30394426796544494</v>
       </c>
       <c r="E31" s="19">
-        <f t="shared" si="29"/>
-        <v>0.34789284418656286</v>
+        <f t="shared" si="27"/>
+        <v>0.34984163789112804</v>
       </c>
       <c r="F31" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G31" s="21">
-        <f t="shared" si="30"/>
-        <v>0.33926938791358691</v>
+        <f t="shared" si="28"/>
+        <v>0.33924303349568063</v>
       </c>
       <c r="H31" s="21">
         <f t="shared" si="0"/>
-        <v>0.34598660552332033</v>
+        <v>0.34623020473639099</v>
       </c>
       <c r="I31" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.33811427413479361</v>
+        <f t="shared" si="29"/>
+        <v>-0.33325146220223512</v>
       </c>
       <c r="J31" s="19">
-        <f t="shared" si="31"/>
-        <v>0.86596775875113285</v>
+        <f t="shared" si="29"/>
+        <v>0.85964645221675395</v>
       </c>
       <c r="K31" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.23811427413480132</v>
+        <f t="shared" si="29"/>
+        <v>-0.24921278106775396</v>
       </c>
       <c r="L31" s="19">
-        <f t="shared" si="31"/>
-        <v>0.99596775875113375</v>
+        <f t="shared" si="29"/>
+        <v>0.99856862152459236</v>
       </c>
       <c r="M31" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N31" s="21">
         <f t="shared" si="1"/>
-        <v>0.10290382773489257</v>
+        <v>0.10066177083362876</v>
       </c>
       <c r="O31" s="21">
         <f t="shared" si="2"/>
-        <v>0.93838785552537152</v>
+        <v>0.93736368845760665</v>
       </c>
       <c r="P31" s="22">
         <f t="shared" si="3"/>
-        <v>8.6311212077945943E-3</v>
+        <v>8.21955669068942E-3</v>
       </c>
       <c r="Q31" s="22">
         <f t="shared" si="4"/>
-        <v>2.6638134572699226E-3</v>
+        <v>2.7705812927878905E-3</v>
       </c>
       <c r="R31" s="22">
         <f t="shared" si="5"/>
-        <v>1.1294934665064517E-2</v>
+        <v>1.0990137983477311E-2</v>
       </c>
       <c r="T31">
         <f t="shared" si="6"/>
-        <v>1.3253011219762367E-2</v>
+        <v>1.2903373400149885E-2</v>
       </c>
       <c r="U31">
         <f t="shared" si="7"/>
-        <v>0.19580765546978496</v>
+        <v>0.1913235416672574</v>
       </c>
       <c r="V31">
         <f t="shared" si="8"/>
-        <v>1.0362691775571947E-2</v>
+        <v>1.0037411752629443E-2</v>
       </c>
       <c r="W31">
         <f t="shared" si="9"/>
-        <v>-9.3224288949256967E-2</v>
+        <v>-9.5272623084786776E-2</v>
       </c>
       <c r="Y31">
         <f t="shared" si="10"/>
-        <v>0.10629652161402842</v>
+        <v>0.10405420116858555</v>
       </c>
       <c r="Z31">
+        <f t="shared" si="31"/>
+        <v>0.33924303349567864</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="32"/>
+        <v>0.34623020473639188</v>
+      </c>
+      <c r="AB31">
         <f t="shared" si="33"/>
-        <v>0.33926938791358496</v>
-      </c>
-      <c r="AA31">
+        <v>0.33924303349568419</v>
+      </c>
+      <c r="AC31">
         <f t="shared" si="34"/>
-        <v>0.34598660552332128</v>
-      </c>
-      <c r="AB31">
-        <f t="shared" si="35"/>
-        <v>0.33926938791359884</v>
-      </c>
-      <c r="AC31">
-        <f t="shared" si="36"/>
-        <v>0.3459866055233185</v>
+        <v>0.34623020473638633</v>
       </c>
       <c r="AE31">
         <f t="shared" si="11"/>
-        <v>6.6431543420028064E-2</v>
+        <v>6.4905178654337273E-2</v>
       </c>
       <c r="AF31">
+        <f t="shared" si="35"/>
+        <v>-3.2320573664374012E-2</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="36"/>
+        <v>6.6241989002346138E-2</v>
+      </c>
+      <c r="AH31">
         <f t="shared" si="12"/>
-        <v>-3.2254355285878687E-2</v>
-      </c>
-      <c r="AG31">
-        <f t="shared" si="13"/>
-        <v>6.6431543420030784E-2</v>
-      </c>
-      <c r="AH31">
-        <f t="shared" si="14"/>
-        <v>-3.225435528587843E-2</v>
+        <v>-3.2986259796418289E-2</v>
       </c>
       <c r="AJ31">
         <f t="shared" si="37"/>
-        <v>-0.37133004584480767</v>
+        <v>-0.36570405152940377</v>
       </c>
       <c r="AK31">
         <f t="shared" si="38"/>
-        <v>0.88209493639407222</v>
+        <v>0.87580673904894091</v>
       </c>
       <c r="AL31">
         <f t="shared" si="39"/>
-        <v>-0.27133004584481674</v>
+        <v>-0.28233377556892703</v>
       </c>
       <c r="AM31">
         <f t="shared" si="40"/>
-        <v>1.012094936394073</v>
+        <v>1.0150617514228015</v>
       </c>
       <c r="AO31">
+        <f t="shared" si="13"/>
+        <v>-6.3758850014323784E-2</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="14"/>
+        <v>-8.1900772428220969E-2</v>
+      </c>
+      <c r="AQ31">
         <f t="shared" si="15"/>
-        <v>-6.6205363299202097E-2</v>
-      </c>
-      <c r="AP31">
+        <v>-0.14565962244254477</v>
+      </c>
+      <c r="AR31">
         <f t="shared" si="16"/>
-        <v>-8.0729228562556057E-2</v>
-      </c>
-      <c r="AQ31">
+        <v>-4.7680271902629523E-2</v>
+      </c>
+      <c r="AS31">
         <f t="shared" si="17"/>
-        <v>-0.14693459186175817</v>
-      </c>
-      <c r="AR31">
+        <v>-9.5136251902807584E-2</v>
+      </c>
+      <c r="AT31">
         <f t="shared" si="18"/>
-        <v>-4.6624597752225105E-2</v>
-      </c>
-      <c r="AS31">
+        <v>-0.14281652380543711</v>
+      </c>
+      <c r="AV31">
         <f t="shared" si="19"/>
-        <v>-9.2848386125959553E-2</v>
-      </c>
-      <c r="AT31">
+        <v>0.05</v>
+      </c>
+      <c r="AW31">
         <f t="shared" si="20"/>
-        <v>-0.13947298387818466</v>
-      </c>
-      <c r="AV31">
+        <v>0.1</v>
+      </c>
+      <c r="AX31">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW31">
+      <c r="AY31">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX31">
+      <c r="BA31" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY31">
+        <v>-7.2829811221272389E-3</v>
+      </c>
+      <c r="BB31" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA31" s="4">
+        <v>-7.1408261902718559E-3</v>
+      </c>
+      <c r="BC31" s="4">
         <f t="shared" si="25"/>
-        <v>-7.3467295930879084E-3</v>
-      </c>
-      <c r="BB31" s="4">
+        <v>-1.4565962244254478E-2</v>
+      </c>
+      <c r="BD31" s="4">
         <f t="shared" si="26"/>
-        <v>-6.9736491939092335E-3</v>
-      </c>
-      <c r="BC31" s="4">
-        <f t="shared" si="27"/>
-        <v>-1.4693459186175817E-2</v>
-      </c>
-      <c r="BD31" s="4">
-        <f t="shared" si="28"/>
-        <v>-1.3947298387818467E-2</v>
+        <v>-1.4281652380543712E-2</v>
       </c>
       <c r="BE31" s="4"/>
       <c r="BF31" s="4">
         <f t="shared" si="41"/>
-        <v>0.18075091645089164</v>
+        <v>0.18061362454378604</v>
       </c>
       <c r="BG31" s="4">
         <f t="shared" si="42"/>
-        <v>0.22743324669023607</v>
+        <v>0.22849123204069993</v>
       </c>
       <c r="BH31" s="4">
         <f t="shared" si="43"/>
-        <v>0.31150183290178324</v>
+        <v>0.31122724908757216</v>
       </c>
       <c r="BI31" s="4">
         <f t="shared" si="44"/>
-        <v>0.3548664933804721</v>
+        <v>0.35698246408139989</v>
       </c>
     </row>
     <row r="32" spans="2:61">
       <c r="B32" s="19">
-        <f t="shared" si="29"/>
-        <v>0.18075091645089164</v>
+        <f t="shared" si="27"/>
+        <v>0.18061362454378604</v>
       </c>
       <c r="C32" s="19">
-        <f t="shared" si="29"/>
-        <v>0.22743324669023607</v>
+        <f t="shared" si="27"/>
+        <v>0.22849123204069993</v>
       </c>
       <c r="D32" s="19">
-        <f t="shared" si="29"/>
-        <v>0.31150183290178324</v>
+        <f t="shared" si="27"/>
+        <v>0.31122724908757216</v>
       </c>
       <c r="E32" s="19">
-        <f t="shared" si="29"/>
-        <v>0.3548664933804721</v>
+        <f t="shared" si="27"/>
+        <v>0.35698246408139989</v>
       </c>
       <c r="F32" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G32" s="21">
-        <f t="shared" si="30"/>
-        <v>0.34018772911272288</v>
+        <f t="shared" si="28"/>
+        <v>0.34015340613594652</v>
       </c>
       <c r="H32" s="21">
         <f t="shared" si="0"/>
-        <v>0.34685831167255898</v>
+        <v>0.34712280801017498</v>
       </c>
       <c r="I32" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.37133004584480767</v>
+        <f t="shared" si="29"/>
+        <v>-0.36570405152940377</v>
       </c>
       <c r="J32" s="19">
-        <f t="shared" si="31"/>
-        <v>0.88209493639407222</v>
+        <f t="shared" si="29"/>
+        <v>0.87580673904894091</v>
       </c>
       <c r="K32" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.27133004584481674</v>
+        <f t="shared" si="29"/>
+        <v>-0.28233377556892703</v>
       </c>
       <c r="L32" s="19">
-        <f t="shared" si="31"/>
-        <v>1.012094936394073</v>
+        <f t="shared" si="29"/>
+        <v>1.0150617514228015</v>
       </c>
       <c r="M32" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N32" s="21">
         <f t="shared" si="1"/>
-        <v>7.956499334496045E-2</v>
+        <v>7.7600028262957088E-2</v>
       </c>
       <c r="O32" s="21">
         <f t="shared" si="2"/>
-        <v>0.95113141416372526</v>
+        <v>0.9502597308619225</v>
       </c>
       <c r="P32" s="22">
         <f t="shared" si="3"/>
-        <v>4.8392882990843924E-3</v>
+        <v>4.5697638211525974E-3</v>
       </c>
       <c r="Q32" s="22">
         <f t="shared" si="4"/>
-        <v>1.5107669649118563E-3</v>
+        <v>1.579288991166834E-3</v>
       </c>
       <c r="R32" s="22">
         <f t="shared" si="5"/>
-        <v>6.3500552639962488E-3</v>
+        <v>6.1490528123194317E-3</v>
       </c>
       <c r="T32">
         <f t="shared" si="6"/>
-        <v>7.8413551308954572E-3</v>
+        <v>7.6010533775785734E-3</v>
       </c>
       <c r="U32">
         <f t="shared" si="7"/>
-        <v>0.14912998668992083</v>
+        <v>0.14520005652591417</v>
       </c>
       <c r="V32">
         <f t="shared" si="8"/>
-        <v>5.6726835472707534E-3</v>
+        <v>5.4542474295578812E-3</v>
       </c>
       <c r="W32">
         <f t="shared" si="9"/>
-        <v>-6.7737171672549529E-2</v>
+        <v>-6.9480538276155052E-2</v>
       </c>
       <c r="Y32">
         <f t="shared" si="10"/>
-        <v>8.2966870636087653E-2</v>
+        <v>8.1001562324316573E-2</v>
       </c>
       <c r="Z32">
+        <f t="shared" si="31"/>
+        <v>0.34015340613594847</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="32"/>
+        <v>0.34712280801017792</v>
+      </c>
+      <c r="AB32">
         <f t="shared" si="33"/>
-        <v>0.34018772911272033</v>
-      </c>
-      <c r="AA32">
+        <v>0.34015340613593459</v>
+      </c>
+      <c r="AC32">
         <f t="shared" si="34"/>
-        <v>0.3468583116725571</v>
-      </c>
-      <c r="AB32">
-        <f t="shared" si="35"/>
-        <v>0.34018772911272865</v>
-      </c>
-      <c r="AC32">
-        <f t="shared" si="36"/>
-        <v>0.34685831167255987</v>
+        <v>0.34712280801016959</v>
       </c>
       <c r="AE32">
         <f t="shared" si="11"/>
-        <v>5.0732191514654378E-2</v>
+        <v>4.9390293798421955E-2</v>
       </c>
       <c r="AF32">
+        <f t="shared" si="35"/>
+        <v>-2.3634041754792317E-2</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="36"/>
+        <v>5.0402251344511886E-2</v>
+      </c>
+      <c r="AH32">
         <f t="shared" si="12"/>
-        <v>-2.3495201003814688E-2</v>
-      </c>
-      <c r="AG32">
-        <f t="shared" si="13"/>
-        <v>5.073219151465562E-2</v>
-      </c>
-      <c r="AH32">
-        <f t="shared" si="14"/>
-        <v>-2.3495201003814879E-2</v>
+        <v>-2.411827954847701E-2</v>
       </c>
       <c r="AJ32">
         <f t="shared" si="37"/>
-        <v>-0.39669614160213484</v>
+        <v>-0.39039919842861476</v>
       </c>
       <c r="AK32">
         <f t="shared" si="38"/>
-        <v>0.89384253689597959</v>
+        <v>0.88762375992633702</v>
       </c>
       <c r="AL32">
         <f t="shared" si="39"/>
-        <v>-0.29669614160214453</v>
+        <v>-0.30753490124118299</v>
       </c>
       <c r="AM32">
         <f t="shared" si="40"/>
-        <v>1.0238425368959805</v>
+        <v>1.02712089119704</v>
       </c>
       <c r="AO32">
+        <f t="shared" si="13"/>
+        <v>-5.3100248953825258E-2</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="14"/>
+        <v>-6.0851523655004479E-2</v>
+      </c>
+      <c r="AQ32">
         <f t="shared" si="15"/>
-        <v>-5.5376444794403859E-2</v>
-      </c>
-      <c r="AP32">
+        <v>-0.11395177260882974</v>
+      </c>
+      <c r="AR32">
         <f t="shared" si="16"/>
-        <v>-5.9750616138011928E-2</v>
-      </c>
-      <c r="AQ32">
+        <v>-4.0994880171782967E-2</v>
+      </c>
+      <c r="AS32">
         <f t="shared" si="17"/>
-        <v>-0.11512706093241579</v>
-      </c>
-      <c r="AR32">
+        <v>-7.0527036872392951E-2</v>
+      </c>
+      <c r="AT32">
         <f t="shared" si="18"/>
-        <v>-4.0463446125413131E-2</v>
-      </c>
-      <c r="AS32">
+        <v>-0.11152191704417591</v>
+      </c>
+      <c r="AV32">
         <f t="shared" si="19"/>
-        <v>-6.8556448455443425E-2</v>
-      </c>
-      <c r="AT32">
+        <v>0.05</v>
+      </c>
+      <c r="AW32">
         <f t="shared" si="20"/>
-        <v>-0.10901989458085656</v>
-      </c>
-      <c r="AV32">
+        <v>0.1</v>
+      </c>
+      <c r="AX32">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW32">
+      <c r="AY32">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX32">
+      <c r="BA32" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY32">
+        <v>-5.6975886304414872E-3</v>
+      </c>
+      <c r="BB32" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA32" s="4">
+        <v>-5.5760958522087962E-3</v>
+      </c>
+      <c r="BC32" s="4">
         <f t="shared" si="25"/>
-        <v>-5.7563530466207893E-3</v>
-      </c>
-      <c r="BB32" s="4">
+        <v>-1.1395177260882974E-2</v>
+      </c>
+      <c r="BD32" s="4">
         <f t="shared" si="26"/>
-        <v>-5.4509947290428285E-3</v>
-      </c>
-      <c r="BC32" s="4">
-        <f t="shared" si="27"/>
-        <v>-1.1512706093241579E-2</v>
-      </c>
-      <c r="BD32" s="4">
-        <f t="shared" si="28"/>
-        <v>-1.0901989458085657E-2</v>
+        <v>-1.1152191704417592E-2</v>
       </c>
       <c r="BE32" s="4"/>
       <c r="BF32" s="4">
         <f t="shared" si="41"/>
-        <v>0.18362909297420205</v>
+        <v>0.1834624188590068</v>
       </c>
       <c r="BG32" s="4">
         <f t="shared" si="42"/>
-        <v>0.23015874405475747</v>
+        <v>0.23127927996680434</v>
       </c>
       <c r="BH32" s="4">
         <f t="shared" si="43"/>
-        <v>0.31725818594840405</v>
+        <v>0.31692483771801366</v>
       </c>
       <c r="BI32" s="4">
         <f t="shared" si="44"/>
-        <v>0.36031748810951492</v>
+        <v>0.36255855993360869</v>
       </c>
     </row>
     <row r="33" spans="2:61">
       <c r="B33" s="19">
-        <f t="shared" si="29"/>
-        <v>0.18362909297420205</v>
+        <f t="shared" si="27"/>
+        <v>0.1834624188590068</v>
       </c>
       <c r="C33" s="19">
-        <f t="shared" si="29"/>
-        <v>0.23015874405475747</v>
+        <f t="shared" si="27"/>
+        <v>0.23127927996680434</v>
       </c>
       <c r="D33" s="19">
-        <f t="shared" si="29"/>
-        <v>0.31725818594840405</v>
+        <f t="shared" si="27"/>
+        <v>0.31692483771801366</v>
       </c>
       <c r="E33" s="19">
-        <f t="shared" si="29"/>
-        <v>0.36031748810951492</v>
+        <f t="shared" si="27"/>
+        <v>0.36255855993360869</v>
       </c>
       <c r="F33" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G33" s="21">
-        <f t="shared" si="30"/>
-        <v>0.34090727324355052</v>
+        <f t="shared" si="28"/>
+        <v>0.34086560471475169</v>
       </c>
       <c r="H33" s="21">
         <f t="shared" si="0"/>
-        <v>0.34753968601368934</v>
+        <v>0.34781981999170108</v>
       </c>
       <c r="I33" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.39669614160213484</v>
+        <f t="shared" si="29"/>
+        <v>-0.39039919842861476</v>
       </c>
       <c r="J33" s="19">
-        <f t="shared" si="31"/>
-        <v>0.89384253689597959</v>
+        <f t="shared" si="29"/>
+        <v>0.88762375992633702</v>
       </c>
       <c r="K33" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.29669614160214453</v>
+        <f t="shared" si="29"/>
+        <v>-0.30753490124118299</v>
       </c>
       <c r="L33" s="19">
-        <f t="shared" si="31"/>
-        <v>1.0238425368959805</v>
+        <f t="shared" si="29"/>
+        <v>1.02712089119704</v>
       </c>
       <c r="M33" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N33" s="21">
         <f t="shared" si="1"/>
-        <v>6.1649716166296359E-2</v>
+        <v>5.9959607156602035E-2</v>
       </c>
       <c r="O33" s="21">
         <f t="shared" si="2"/>
-        <v>0.96054333576259432</v>
+        <v>0.95981341317234259</v>
       </c>
       <c r="P33" s="22">
         <f t="shared" si="3"/>
-        <v>2.6676931800589752E-3</v>
+        <v>2.4959623472420012E-3</v>
       </c>
       <c r="Q33" s="22">
         <f t="shared" si="4"/>
-        <v>8.6769506799525432E-4</v>
+        <v>9.1123002430369942E-4</v>
       </c>
       <c r="R33" s="22">
         <f t="shared" si="5"/>
-        <v>3.5353882480542295E-3</v>
+        <v>3.4071923715457007E-3</v>
       </c>
       <c r="T33">
         <f t="shared" si="6"/>
-        <v>4.6683825713801563E-3</v>
+        <v>4.5063845146777401E-3</v>
       </c>
       <c r="U33">
         <f t="shared" si="7"/>
-        <v>0.11329943233259268</v>
+        <v>0.10991921431320394</v>
       </c>
       <c r="V33">
         <f t="shared" si="8"/>
-        <v>3.0462549633061158E-3</v>
+        <v>2.9034606349925521E-3</v>
       </c>
       <c r="W33">
         <f t="shared" si="9"/>
-        <v>-4.8913328474811363E-2</v>
+        <v>-5.0373173655314865E-2</v>
       </c>
       <c r="Y33">
         <f t="shared" si="10"/>
-        <v>6.5058788898731873E-2</v>
+        <v>6.3368263203749553E-2</v>
       </c>
       <c r="Z33">
+        <f t="shared" si="31"/>
+        <v>0.3408656047147518</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="32"/>
+        <v>0.34781981999170153</v>
+      </c>
+      <c r="AB33">
         <f t="shared" si="33"/>
-        <v>0.34090727324355141</v>
-      </c>
-      <c r="AA33">
+        <v>0.34086560471473515</v>
+      </c>
+      <c r="AC33">
         <f t="shared" si="34"/>
-        <v>0.34753968601368979</v>
-      </c>
-      <c r="AB33">
-        <f t="shared" si="35"/>
-        <v>0.34090727324356251</v>
-      </c>
-      <c r="AC33">
-        <f t="shared" si="36"/>
-        <v>0.34753968601368701</v>
+        <v>0.34781981999170153</v>
       </c>
       <c r="AE33">
         <f t="shared" si="11"/>
-        <v>3.8624600536546434E-2</v>
+        <v>3.746767945664066E-2</v>
       </c>
       <c r="AF33">
+        <f t="shared" si="35"/>
+        <v>-1.7170482299419268E-2</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="36"/>
+        <v>3.8232081336047857E-2</v>
+      </c>
+      <c r="AH33">
         <f t="shared" si="12"/>
-        <v>-1.6999322820020413E-2</v>
-      </c>
-      <c r="AG33">
-        <f t="shared" si="13"/>
-        <v>3.8624600536547697E-2</v>
-      </c>
-      <c r="AH33">
-        <f t="shared" si="14"/>
-        <v>-1.6999322820020278E-2</v>
+        <v>-1.7520788193202338E-2</v>
       </c>
       <c r="AJ33">
         <f t="shared" si="37"/>
-        <v>-0.41600844187040809</v>
+        <v>-0.40913303815693508</v>
       </c>
       <c r="AK33">
         <f t="shared" si="38"/>
-        <v>0.90234219830598983</v>
+        <v>0.89620900107604662</v>
       </c>
       <c r="AL33">
         <f t="shared" si="39"/>
-        <v>-0.31600844187041838</v>
+        <v>-0.3266509419092069</v>
       </c>
       <c r="AM33">
         <f t="shared" si="40"/>
-        <v>1.0323421983059906</v>
+        <v>1.0358812852936412</v>
       </c>
       <c r="AO33">
+        <f t="shared" si="13"/>
+        <v>-4.2912373159777938E-2</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="14"/>
+        <v>-4.471242579935289E-2</v>
+      </c>
+      <c r="AQ33">
         <f t="shared" si="15"/>
-        <v>-4.4945447652051683E-2</v>
-      </c>
-      <c r="AP33">
+        <v>-8.7624798959130834E-2</v>
+      </c>
+      <c r="AR33">
         <f t="shared" si="16"/>
-        <v>-4.3720813611951743E-2</v>
-      </c>
-      <c r="AQ33">
+        <v>-3.3803994718319602E-2</v>
+      </c>
+      <c r="AS33">
         <f t="shared" si="17"/>
-        <v>-8.8666261264003426E-2</v>
-      </c>
-      <c r="AR33">
+        <v>-5.1739339017270257E-2</v>
+      </c>
+      <c r="AT33">
         <f t="shared" si="18"/>
-        <v>-3.3615504418793511E-2</v>
-      </c>
-      <c r="AS33">
+        <v>-8.5543333735589866E-2</v>
+      </c>
+      <c r="AV33">
         <f t="shared" si="19"/>
-        <v>-5.0079546313677267E-2</v>
-      </c>
-      <c r="AT33">
+        <v>0.05</v>
+      </c>
+      <c r="AW33">
         <f t="shared" si="20"/>
-        <v>-8.3695050732470772E-2</v>
-      </c>
-      <c r="AV33">
+        <v>0.1</v>
+      </c>
+      <c r="AX33">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW33">
+      <c r="AY33">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX33">
+      <c r="BA33" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY33">
+        <v>-4.3812399479565417E-3</v>
+      </c>
+      <c r="BB33" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA33" s="4">
+        <v>-4.2771666867794933E-3</v>
+      </c>
+      <c r="BC33" s="4">
         <f t="shared" si="25"/>
-        <v>-4.4333130632001711E-3</v>
-      </c>
-      <c r="BB33" s="4">
+        <v>-8.7624798959130834E-3</v>
+      </c>
+      <c r="BD33" s="4">
         <f t="shared" si="26"/>
-        <v>-4.1847525366235389E-3</v>
-      </c>
-      <c r="BC33" s="4">
-        <f t="shared" si="27"/>
-        <v>-8.8666261264003423E-3</v>
-      </c>
-      <c r="BD33" s="4">
-        <f t="shared" si="28"/>
-        <v>-8.3695050732470778E-3</v>
+        <v>-8.5543333735589866E-3</v>
       </c>
       <c r="BE33" s="4"/>
       <c r="BF33" s="4">
         <f t="shared" si="41"/>
-        <v>0.18584574950580213</v>
+        <v>0.18565303883298506</v>
       </c>
       <c r="BG33" s="4">
         <f t="shared" si="42"/>
-        <v>0.23225112032306924</v>
+        <v>0.2334178633101941</v>
       </c>
       <c r="BH33" s="4">
         <f t="shared" si="43"/>
-        <v>0.32169149901160421</v>
+        <v>0.32130607766597019</v>
       </c>
       <c r="BI33" s="4">
         <f t="shared" si="44"/>
-        <v>0.36450224064613845</v>
+        <v>0.36683572662038821</v>
       </c>
     </row>
     <row r="34" spans="2:61">
       <c r="B34" s="19">
-        <f t="shared" si="29"/>
-        <v>0.18584574950580213</v>
+        <f t="shared" si="27"/>
+        <v>0.18565303883298506</v>
       </c>
       <c r="C34" s="19">
-        <f t="shared" si="29"/>
-        <v>0.23225112032306924</v>
+        <f t="shared" si="27"/>
+        <v>0.2334178633101941</v>
       </c>
       <c r="D34" s="19">
-        <f t="shared" si="29"/>
-        <v>0.32169149901160421</v>
+        <f t="shared" si="27"/>
+        <v>0.32130607766597019</v>
       </c>
       <c r="E34" s="19">
-        <f t="shared" si="29"/>
-        <v>0.36450224064613845</v>
+        <f t="shared" si="27"/>
+        <v>0.36683572662038821</v>
       </c>
       <c r="F34" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G34" s="21">
-        <f t="shared" si="30"/>
-        <v>0.34146143737645052</v>
+        <f t="shared" si="28"/>
+        <v>0.34141325970824626</v>
       </c>
       <c r="H34" s="21">
         <f t="shared" si="0"/>
-        <v>0.3480627800807673</v>
+        <v>0.34835446582754853</v>
       </c>
       <c r="I34" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.41600844187040809</v>
+        <f t="shared" si="29"/>
+        <v>-0.40913303815693508</v>
       </c>
       <c r="J34" s="19">
-        <f t="shared" si="31"/>
-        <v>0.90234219830598983</v>
+        <f t="shared" si="29"/>
+        <v>0.89620900107604662</v>
       </c>
       <c r="K34" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.31600844187041838</v>
+        <f t="shared" si="29"/>
+        <v>-0.3266509419092069</v>
       </c>
       <c r="L34" s="19">
-        <f t="shared" si="31"/>
-        <v>1.0323421983059906</v>
+        <f t="shared" si="29"/>
+        <v>1.0358812852936412</v>
       </c>
       <c r="M34" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N34" s="21">
         <f t="shared" si="1"/>
-        <v>4.7958382671783484E-2</v>
+        <v>4.65262414076551E-2</v>
       </c>
       <c r="O34" s="21">
         <f t="shared" si="2"/>
-        <v>0.9674349595760634</v>
+        <v>0.96683150823646513</v>
       </c>
       <c r="P34" s="22">
         <f t="shared" si="3"/>
-        <v>1.4408388150575525E-3</v>
+        <v>1.3341663113702979E-3</v>
       </c>
       <c r="Q34" s="22">
         <f t="shared" si="4"/>
-        <v>5.0918104933389237E-4</v>
+        <v>5.3677901059698263E-4</v>
       </c>
       <c r="R34" s="22">
         <f t="shared" si="5"/>
-        <v>1.950019864391445E-3</v>
+        <v>1.8709453219672807E-3</v>
       </c>
       <c r="T34">
         <f t="shared" si="6"/>
-        <v>2.8091875178271148E-3</v>
+        <v>2.7014701501203828E-3</v>
       </c>
       <c r="U34">
         <f t="shared" si="7"/>
-        <v>8.5916765343566973E-2</v>
+        <v>8.3052482815310205E-2</v>
       </c>
       <c r="V34">
         <f t="shared" si="8"/>
-        <v>1.5987190559127128E-3</v>
+        <v>1.5075754866965831E-3</v>
       </c>
       <c r="W34">
         <f t="shared" si="9"/>
-        <v>-3.5130080847873224E-2</v>
+        <v>-3.6336983527069752E-2</v>
       </c>
       <c r="Y34">
         <f t="shared" si="10"/>
-        <v>5.1372997045548013E-2</v>
+        <v>4.9940374004737553E-2</v>
       </c>
       <c r="Z34">
+        <f t="shared" si="31"/>
+        <v>0.34141325970824532</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="32"/>
+        <v>0.34835446582755225</v>
+      </c>
+      <c r="AB34">
         <f t="shared" si="33"/>
-        <v>0.34146143737645296</v>
-      </c>
-      <c r="AA34">
+        <v>0.34141325970824532</v>
+      </c>
+      <c r="AC34">
         <f t="shared" si="34"/>
-        <v>0.34806278008077118</v>
-      </c>
-      <c r="AB34">
-        <f t="shared" si="35"/>
-        <v>0.34146143737645573</v>
-      </c>
-      <c r="AC34">
-        <f t="shared" si="36"/>
-        <v>0.34806278008074898</v>
+        <v>0.34835446582754948</v>
       </c>
       <c r="AE34">
         <f t="shared" si="11"/>
-        <v>2.9337262188949796E-2</v>
+        <v>2.8355218884838086E-2</v>
       </c>
       <c r="AF34">
+        <f t="shared" si="35"/>
+        <v>-1.2405927993941697E-2</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="36"/>
+        <v>2.893170328677935E-2</v>
+      </c>
+      <c r="AH34">
         <f t="shared" si="12"/>
-        <v>-1.2227473604373009E-2</v>
-      </c>
-      <c r="AG34">
-        <f t="shared" si="13"/>
-        <v>2.9337262188950036E-2</v>
-      </c>
-      <c r="AH34">
-        <f t="shared" si="14"/>
-        <v>-1.222747360437223E-2</v>
+        <v>-1.2658150486356849E-2</v>
       </c>
       <c r="AJ34">
         <f t="shared" si="37"/>
-        <v>-0.430677072964883</v>
+        <v>-0.42331064759935411</v>
       </c>
       <c r="AK34">
         <f t="shared" si="38"/>
-        <v>0.90845593510817635</v>
+        <v>0.90241196507301746</v>
       </c>
       <c r="AL34">
         <f t="shared" si="39"/>
-        <v>-0.3306770729648934</v>
+        <v>-0.34111679355259655</v>
       </c>
       <c r="AM34">
         <f t="shared" si="40"/>
-        <v>1.0384559351081768</v>
+        <v>1.0422103605368196</v>
       </c>
       <c r="AO34">
+        <f t="shared" si="13"/>
+        <v>-3.3979514620704504E-2</v>
+      </c>
+      <c r="AP34">
+        <f t="shared" si="14"/>
+        <v>-3.2565531708911945E-2</v>
+      </c>
+      <c r="AQ34">
         <f t="shared" si="15"/>
-        <v>-3.5742099681122776E-2</v>
-      </c>
-      <c r="AP34">
+        <v>-6.6545046329616442E-2</v>
+      </c>
+      <c r="AR34">
         <f t="shared" si="16"/>
-        <v>-3.1699354378937075E-2</v>
-      </c>
-      <c r="AQ34">
+        <v>-2.7129171739519297E-2</v>
+      </c>
+      <c r="AS34">
         <f t="shared" si="17"/>
-        <v>-6.7441454060059858E-2</v>
-      </c>
-      <c r="AR34">
+        <v>-3.7640801199714885E-2</v>
+      </c>
+      <c r="AT34">
         <f t="shared" si="18"/>
-        <v>-2.715042314676696E-2</v>
-      </c>
-      <c r="AS34">
+        <v>-6.4769972939234186E-2</v>
+      </c>
+      <c r="AV34">
         <f t="shared" si="19"/>
-        <v>-3.626626488916062E-2</v>
-      </c>
-      <c r="AT34">
+        <v>0.05</v>
+      </c>
+      <c r="AW34">
         <f t="shared" si="20"/>
-        <v>-6.3416688035927579E-2</v>
-      </c>
-      <c r="AV34">
+        <v>0.1</v>
+      </c>
+      <c r="AX34">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW34">
+      <c r="AY34">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX34">
+      <c r="BA34" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY34">
+        <v>-3.3272523164808222E-3</v>
+      </c>
+      <c r="BB34" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA34" s="4">
+        <v>-3.2384986469617093E-3</v>
+      </c>
+      <c r="BC34" s="4">
         <f t="shared" si="25"/>
-        <v>-3.3720727030029929E-3</v>
-      </c>
-      <c r="BB34" s="4">
+        <v>-6.6545046329616444E-3</v>
+      </c>
+      <c r="BD34" s="4">
         <f t="shared" si="26"/>
-        <v>-3.1708344017963791E-3</v>
-      </c>
-      <c r="BC34" s="4">
-        <f t="shared" si="27"/>
-        <v>-6.7441454060059858E-3</v>
-      </c>
-      <c r="BD34" s="4">
-        <f t="shared" si="28"/>
-        <v>-6.3416688035927583E-3</v>
+        <v>-6.4769972939234186E-3</v>
       </c>
       <c r="BE34" s="4"/>
       <c r="BF34" s="4">
         <f t="shared" si="41"/>
-        <v>0.18753178585730362</v>
+        <v>0.18731666499122548</v>
       </c>
       <c r="BG34" s="4">
         <f t="shared" si="42"/>
-        <v>0.23383653752396744</v>
+        <v>0.23503711263367494</v>
       </c>
       <c r="BH34" s="4">
         <f t="shared" si="43"/>
-        <v>0.3250635717146072</v>
+        <v>0.32463332998245104</v>
       </c>
       <c r="BI34" s="4">
         <f t="shared" si="44"/>
-        <v>0.36767307504793484</v>
+        <v>0.3700742252673499</v>
       </c>
     </row>
     <row r="35" spans="2:61">
       <c r="B35" s="19">
-        <f t="shared" si="29"/>
-        <v>0.18753178585730362</v>
+        <f t="shared" si="27"/>
+        <v>0.18731666499122548</v>
       </c>
       <c r="C35" s="19">
-        <f t="shared" si="29"/>
-        <v>0.23383653752396744</v>
+        <f t="shared" si="27"/>
+        <v>0.23503711263367494</v>
       </c>
       <c r="D35" s="19">
-        <f t="shared" si="29"/>
-        <v>0.3250635717146072</v>
+        <f t="shared" si="27"/>
+        <v>0.32463332998245104</v>
       </c>
       <c r="E35" s="19">
-        <f t="shared" si="29"/>
-        <v>0.36767307504793484</v>
+        <f t="shared" si="27"/>
+        <v>0.3700742252673499</v>
       </c>
       <c r="F35" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G35" s="21">
-        <f t="shared" si="30"/>
-        <v>0.34188294646432588</v>
+        <f t="shared" si="28"/>
+        <v>0.34182916624780635</v>
       </c>
       <c r="H35" s="21">
         <f t="shared" si="0"/>
-        <v>0.34845913438099185</v>
+        <v>0.34875927815841873</v>
       </c>
       <c r="I35" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.430677072964883</v>
+        <f t="shared" si="29"/>
+        <v>-0.42331064759935411</v>
       </c>
       <c r="J35" s="19">
-        <f t="shared" si="31"/>
-        <v>0.90845593510817635</v>
+        <f t="shared" si="29"/>
+        <v>0.90241196507301746</v>
       </c>
       <c r="K35" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.3306770729648934</v>
+        <f t="shared" si="29"/>
+        <v>-0.34111679355259655</v>
       </c>
       <c r="L35" s="19">
-        <f t="shared" si="31"/>
-        <v>1.0384559351081768</v>
+        <f t="shared" si="29"/>
+        <v>1.0422103605368196</v>
       </c>
       <c r="M35" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N35" s="21">
         <f t="shared" si="1"/>
-        <v>3.7531406715147486E-2</v>
+        <v>3.6332427580175908E-2</v>
       </c>
       <c r="O35" s="21">
         <f t="shared" si="2"/>
-        <v>0.97244504806838661</v>
+        <v>0.97195126266300069</v>
       </c>
       <c r="P35" s="22">
         <f t="shared" si="3"/>
-        <v>7.5797835571486801E-4</v>
+        <v>6.933967422652087E-4</v>
       </c>
       <c r="Q35" s="22">
         <f t="shared" si="4"/>
-        <v>3.0817633732125644E-4</v>
+        <v>3.2575691945999253E-4</v>
       </c>
       <c r="R35" s="22">
         <f t="shared" si="5"/>
-        <v>1.0661546930361245E-3</v>
+        <v>1.0191536617252012E-3</v>
       </c>
       <c r="T35">
         <f t="shared" si="6"/>
-        <v>1.7167828273390742E-3</v>
+        <v>1.6458022133287195E-3</v>
       </c>
       <c r="U35">
         <f t="shared" si="7"/>
-        <v>6.5062813430294977E-2</v>
+        <v>6.2664855160351834E-2</v>
       </c>
       <c r="V35">
         <f t="shared" si="8"/>
-        <v>8.150556544038567E-4</v>
+        <v>7.5817891498521518E-4</v>
       </c>
       <c r="W35">
         <f t="shared" si="9"/>
-        <v>-2.5109903863226781E-2</v>
+        <v>-2.6097474673998599E-2</v>
       </c>
       <c r="Y35">
         <f t="shared" si="10"/>
-        <v>4.0950236179790767E-2</v>
+        <v>3.9750719242653942E-2</v>
       </c>
       <c r="Z35">
+        <f t="shared" si="31"/>
+        <v>0.34182916624780346</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="32"/>
+        <v>0.34875927815841701</v>
+      </c>
+      <c r="AB35">
         <f t="shared" si="33"/>
-        <v>0.34188294646432804</v>
-      </c>
-      <c r="AA35">
+        <v>0.34182916624780901</v>
+      </c>
+      <c r="AC35">
         <f t="shared" si="34"/>
-        <v>0.34845913438099618</v>
-      </c>
-      <c r="AB35">
-        <f t="shared" si="35"/>
-        <v>0.34188294646431139</v>
-      </c>
-      <c r="AC35">
-        <f t="shared" si="36"/>
-        <v>0.34845913438097398</v>
+        <v>0.34875927815840591</v>
       </c>
       <c r="AE35">
         <f t="shared" si="11"/>
-        <v>2.22438663608081E-2</v>
+        <v>2.1420675192502431E-2</v>
       </c>
       <c r="AF35">
+        <f t="shared" si="35"/>
+        <v>-8.9208780089862529E-3</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="36"/>
+        <v>2.1854949651626057E-2</v>
+      </c>
+      <c r="AH35">
         <f t="shared" si="12"/>
-        <v>-8.7497753645700369E-3</v>
-      </c>
-      <c r="AG35">
-        <f t="shared" si="13"/>
-        <v>2.2243866360807017E-2</v>
-      </c>
-      <c r="AH35">
-        <f t="shared" si="14"/>
-        <v>-8.7497753645694783E-3</v>
+        <v>-9.1017364290610307E-3</v>
       </c>
       <c r="AJ35">
         <f t="shared" si="37"/>
-        <v>-0.44179900614528705</v>
+        <v>-0.43402098519560534</v>
       </c>
       <c r="AK35">
         <f t="shared" si="38"/>
-        <v>0.91283082279046135</v>
+        <v>0.90687240407751057</v>
       </c>
       <c r="AL35">
         <f t="shared" si="39"/>
-        <v>-0.3417990061452969</v>
+        <v>-0.35204426837840957</v>
       </c>
       <c r="AM35">
         <f t="shared" si="40"/>
-        <v>1.0428308227904615</v>
+        <v>1.0467612287513501</v>
       </c>
       <c r="AO35">
+        <f t="shared" si="13"/>
+        <v>-2.6526700419648261E-2</v>
+      </c>
+      <c r="AP35">
+        <f t="shared" si="14"/>
+        <v>-2.3550673404006382E-2</v>
+      </c>
+      <c r="AQ35">
         <f t="shared" si="15"/>
-        <v>-2.8021062047019721E-2</v>
-      </c>
-      <c r="AP35">
+        <v>-5.0077373823654639E-2</v>
+      </c>
+      <c r="AR35">
         <f t="shared" si="16"/>
-        <v>-2.2811241194544096E-2</v>
-      </c>
-      <c r="AQ35">
+        <v>-2.13760344607371E-2</v>
+      </c>
+      <c r="AS35">
         <f t="shared" si="17"/>
-        <v>-5.083230324156382E-2</v>
-      </c>
-      <c r="AR35">
+        <v>-2.7199058489088598E-2</v>
+      </c>
+      <c r="AT35">
         <f t="shared" si="18"/>
-        <v>-2.1514780703990898E-2</v>
-      </c>
-      <c r="AS35">
+        <v>-4.8575092949825698E-2</v>
+      </c>
+      <c r="AV35">
         <f t="shared" si="19"/>
-        <v>-2.6075528696763588E-2</v>
-      </c>
-      <c r="AT35">
+        <v>0.05</v>
+      </c>
+      <c r="AW35">
         <f t="shared" si="20"/>
-        <v>-4.7590309400754482E-2</v>
-      </c>
-      <c r="AV35">
+        <v>0.1</v>
+      </c>
+      <c r="AX35">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW35">
+      <c r="AY35">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX35">
+      <c r="BA35" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY35">
+        <v>-2.5038686911827319E-3</v>
+      </c>
+      <c r="BB35" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA35" s="4">
+        <v>-2.428754647491285E-3</v>
+      </c>
+      <c r="BC35" s="4">
         <f t="shared" si="25"/>
-        <v>-2.5416151620781913E-3</v>
-      </c>
-      <c r="BB35" s="4">
+        <v>-5.0077373823654639E-3</v>
+      </c>
+      <c r="BD35" s="4">
         <f t="shared" si="26"/>
-        <v>-2.3795154700377245E-3</v>
-      </c>
-      <c r="BC35" s="4">
-        <f t="shared" si="27"/>
-        <v>-5.0832303241563825E-3</v>
-      </c>
-      <c r="BD35" s="4">
-        <f t="shared" si="28"/>
-        <v>-4.7590309400754489E-3</v>
+        <v>-4.8575092949825699E-3</v>
       </c>
       <c r="BE35" s="4"/>
       <c r="BF35" s="4">
         <f t="shared" si="41"/>
-        <v>0.18880259343834271</v>
+        <v>0.18856859933681686</v>
       </c>
       <c r="BG35" s="4">
         <f t="shared" si="42"/>
-        <v>0.2350262952589863</v>
+        <v>0.23625148995742057</v>
       </c>
       <c r="BH35" s="4">
         <f t="shared" si="43"/>
-        <v>0.32760518687668538</v>
+        <v>0.32713719867363378</v>
       </c>
       <c r="BI35" s="4">
         <f t="shared" si="44"/>
-        <v>0.37005259051797257</v>
+        <v>0.37250297991484116</v>
       </c>
     </row>
     <row r="36" spans="2:61">
       <c r="B36" s="19">
-        <f t="shared" si="29"/>
-        <v>0.18880259343834271</v>
+        <f t="shared" si="27"/>
+        <v>0.18856859933681686</v>
       </c>
       <c r="C36" s="19">
-        <f t="shared" si="29"/>
-        <v>0.2350262952589863</v>
+        <f t="shared" si="27"/>
+        <v>0.23625148995742057</v>
       </c>
       <c r="D36" s="19">
-        <f t="shared" si="29"/>
-        <v>0.32760518687668538</v>
+        <f t="shared" si="27"/>
+        <v>0.32713719867363378</v>
       </c>
       <c r="E36" s="19">
-        <f t="shared" si="29"/>
-        <v>0.37005259051797257</v>
+        <f t="shared" si="27"/>
+        <v>0.37250297991484116</v>
       </c>
       <c r="F36" s="20">
         <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="G36" s="21">
-        <f t="shared" si="30"/>
-        <v>0.34220064835958569</v>
+        <f t="shared" si="28"/>
+        <v>0.34214214983420421</v>
       </c>
       <c r="H36" s="21">
         <f t="shared" si="0"/>
-        <v>0.34875657381474656</v>
+        <v>0.34906287248935514</v>
       </c>
       <c r="I36" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.44179900614528705</v>
+        <f t="shared" si="29"/>
+        <v>-0.43402098519560534</v>
       </c>
       <c r="J36" s="19">
-        <f t="shared" si="31"/>
-        <v>0.91283082279046135</v>
+        <f t="shared" si="29"/>
+        <v>0.90687240407751057</v>
       </c>
       <c r="K36" s="19">
-        <f t="shared" si="31"/>
-        <v>-0.3417990061452969</v>
+        <f t="shared" si="29"/>
+        <v>-0.35204426837840957</v>
       </c>
       <c r="L36" s="19">
-        <f t="shared" si="31"/>
-        <v>1.0428308227904615</v>
+        <f t="shared" si="29"/>
+        <v>1.0467612287513501</v>
       </c>
       <c r="M36" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
       <c r="N36" s="21">
         <f t="shared" si="1"/>
-        <v>2.9611443335942955E-2</v>
+        <v>2.8617543488435149E-2</v>
       </c>
       <c r="O36" s="21">
         <f t="shared" si="2"/>
-        <v>0.97606540422632437</v>
+        <v>0.97566475527482588</v>
       </c>
       <c r="P36" s="22">
         <f t="shared" si="3"/>
-        <v>3.8460870971890126E-4</v>
+        <v>3.4661292554377394E-4</v>
       </c>
       <c r="Q36" s="22">
         <f t="shared" si="4"/>
-        <v>1.9417295937573838E-4</v>
+        <v>2.054992413306322E-4</v>
       </c>
       <c r="R36" s="22">
         <f t="shared" si="5"/>
-        <v>5.7878166909463961E-4</v>
+        <v>5.5211216687440611E-4</v>
       </c>
       <c r="T36">
         <f t="shared" si="6"/>
-        <v>1.0710105358134989E-3</v>
+        <v>1.0244630366431093E-3</v>
       </c>
       <c r="U36">
         <f t="shared" si="7"/>
-        <v>4.9222886671885929E-2</v>
+        <v>4.7235086976870316E-2</v>
       </c>
       <c r="V36">
         <f t="shared" si="8"/>
-        <v>4.0008975362112721E-4</v>
+        <v>3.6540727237092382E-4</v>
       </c>
       <c r="W36">
         <f t="shared" si="9"/>
-        <v>-1.786919154735124E-2</v>
+        <v>-1.8670489450348229E-2</v>
       </c>
       <c r="Y36">
         <f t="shared" si="10"/>
-        <v>3.3033449819538763E-2</v>
+        <v>3.2038964986777219E-2</v>
       </c>
       <c r="Z36">
+        <f t="shared" si="31"/>
+        <v>0.34214214983420699</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="32"/>
+        <v>0.34906287248935852</v>
+      </c>
+      <c r="AB36">
         <f t="shared" si="33"/>
-        <v>0.34220064835958075</v>
-      </c>
-      <c r="AA36">
+        <v>0.34214214983421254</v>
+      </c>
+      <c r="AC36">
         <f t="shared" si="34"/>
-        <v>0.34875657381474579</v>
-      </c>
-      <c r="AB36">
-        <f t="shared" si="35"/>
-        <v>0.34220064835959185</v>
-      </c>
-      <c r="AC36">
-        <f t="shared" si="36"/>
-        <v>0.34875657381474579</v>
+        <v>0.34906287248934742</v>
       </c>
       <c r="AE36">
         <f t="shared" si="11"/>
-        <v>1.684410373324953E-2</v>
+        <v>1.6161114205872164E-2</v>
       </c>
       <c r="AF36">
+        <f t="shared" si="35"/>
+        <v>-6.3879613989991282E-3</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="36"/>
+        <v>1.6488015142431041E-2</v>
+      </c>
+      <c r="AH36">
         <f t="shared" si="12"/>
-        <v>-6.2319980208936339E-3</v>
-      </c>
-      <c r="AG36">
-        <f t="shared" si="13"/>
-        <v>1.6844103733250078E-2</v>
-      </c>
-      <c r="AH36">
-        <f t="shared" si="14"/>
-        <v>-6.2319980208936339E-3</v>
+        <v>-6.5171746783206103E-3</v>
       </c>
       <c r="AJ36">
         <f t="shared" si="37"/>
-        <v>-0.45022105801191181</v>
+        <v>-0.44210154229854143</v>
       </c>
       <c r="AK36">
         <f t="shared" si="38"/>
-        <v>0.91594682180090814</v>
+        <v>0.91006638477701018</v>
       </c>
       <c r="AL36">
         <f t="shared" si="39"/>
-        <v>-0.35022105801192194</v>
+        <v>-0.36028827594962509</v>
       </c>
       <c r="AM36">
         <f t="shared" si="40"/>
-        <v>1.0459468218009083</v>
+        <v>1.0500198160905105</v>
       </c>
       <c r="AO36">
+        <f t="shared" si="13"/>
+        <v>-2.050101898550136E-2</v>
+      </c>
+      <c r="AP36">
+        <f t="shared" si="14"/>
+        <v>-1.6931751653141099E-2</v>
+      </c>
+      <c r="AQ36">
         <f t="shared" si="15"/>
-        <v>-2.1746622411241302E-2</v>
-      </c>
-      <c r="AP36">
+        <v>-3.7432770638642462E-2</v>
+      </c>
+      <c r="AR36">
         <f t="shared" si="16"/>
-        <v>-1.631154882276899E-2</v>
-      </c>
-      <c r="AQ36">
+        <v>-1.6628841636562853E-2</v>
+      </c>
+      <c r="AS36">
         <f t="shared" si="17"/>
-        <v>-3.8058171234010292E-2</v>
-      </c>
-      <c r="AR36">
+        <v>-1.9543544478435631E-2</v>
+      </c>
+      <c r="AT36">
         <f t="shared" si="18"/>
-        <v>-1.6824333744053191E-2</v>
-      </c>
-      <c r="AS36">
+        <v>-3.6172386114998484E-2</v>
+      </c>
+      <c r="AV36">
         <f t="shared" si="19"/>
-        <v>-1.8634543723924653E-2</v>
-      </c>
-      <c r="AT36">
+        <v>0.05</v>
+      </c>
+      <c r="AW36">
         <f t="shared" si="20"/>
-        <v>-3.5458877467977844E-2</v>
-      </c>
-      <c r="AV36">
+        <v>0.1</v>
+      </c>
+      <c r="AX36">
         <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AW36">
+      <c r="AY36">
         <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AX36">
+      <c r="BA36" s="4">
         <f t="shared" si="23"/>
-        <v>0.05</v>
-      </c>
-      <c r="AY36">
+        <v>-1.8716385319321233E-3</v>
+      </c>
+      <c r="BB36" s="4">
         <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="BA36" s="4">
+        <v>-1.8086193057499243E-3</v>
+      </c>
+      <c r="BC36" s="4">
         <f t="shared" si="25"/>
-        <v>-1.9029085617005147E-3</v>
-      </c>
-      <c r="BB36" s="4">
+        <v>-3.7432770638642465E-3</v>
+      </c>
+      <c r="BD36" s="4">
         <f t="shared" si="26"/>
-        <v>-1.7729438733988922E-3</v>
-      </c>
-      <c r="BC36" s="4">
-        <f t="shared" si="27"/>
-        <v>-3.8058171234010294E-3</v>
-      </c>
-      <c r="BD36" s="4">
-        <f t="shared" si="28"/>
-        <v>-3.5458877467977844E-3</v>
+        <v>-3.6172386114998486E-3</v>
       </c>
       <c r="BE36" s="4"/>
       <c r="BF36" s="4">
         <f t="shared" si="41"/>
-        <v>0.18975404771919296</v>
+        <v>0.18950441860278291</v>
       </c>
       <c r="BG36" s="4">
         <f t="shared" si="42"/>
-        <v>0.23591276719568574</v>
+        <v>0.23715579961029554</v>
       </c>
       <c r="BH36" s="4">
         <f t="shared" si="43"/>
-        <v>0.32950809543838588</v>
+        <v>0.3290088372055659</v>
       </c>
       <c r="BI36" s="4">
         <f t="shared" si="44"/>
-        <v>0.37182553439137145</v>
+        <v>0.3743115992205911</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:R22"/>
     <mergeCell ref="T22:W22"/>
     <mergeCell ref="BF22:BI22"/>
     <mergeCell ref="Y22:AC22"/>
@@ -11297,6 +11292,11 @@
     <mergeCell ref="AO22:AT22"/>
     <mergeCell ref="AV22:AY22"/>
     <mergeCell ref="BA22:BD22"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:R22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>